<commit_message>
add [AssemRepo, csv] : Assembles Parts & add ik setting.
</commit_message>
<xml_diff>
--- a/gameCSV/Actor_RobotObj_01.xlsx
+++ b/gameCSV/Actor_RobotObj_01.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltz\Documents\CppProjects\GitManagements\QuantumCoreRobotReMake\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltz\Documents\CppProjects\GitManagements\QuantumCoreRobotReMake\gameCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{C9554B95-70B5-4E00-9A3C-96780F06325F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{104B69C7-339F-4A8C-A822-2F0B79754EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23535" yWindow="4905" windowWidth="17220" windowHeight="10980" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
+    <workbookView xWindow="-16800" yWindow="2445" windowWidth="17160" windowHeight="10980" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
   </bookViews>
   <sheets>
     <sheet name="Actor_RobotObj_01" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
   <si>
     <t>id</t>
     <phoneticPr fontId="1"/>
@@ -103,39 +103,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>obj1</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>obj3</t>
-  </si>
-  <si>
-    <t>obj4</t>
-  </si>
-  <si>
-    <t>obj5</t>
-  </si>
-  <si>
-    <t>obj2</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>obj3</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>obj4</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>obj5</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>obj6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>rot axis:</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -144,23 +111,7 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>root</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>objEE01</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>obj6</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t xml:space="preserve"> IK object</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
-    <t>target01</t>
+    <t>LB01</t>
     <phoneticPr fontId="1"/>
   </si>
   <si>
@@ -168,7 +119,123 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>IK target</t>
+    <t>lb100</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BD01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>bd200</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RA01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ra300</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RA02</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RA03</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LA01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>la400</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LA02</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LA03</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HE01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>HE02</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>he500</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>he501</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RL01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rl600</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RL02</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RL03</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>rl601</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LL01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ll700</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LL02</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LL03</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ll701</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RATA01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>non</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>ra301</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>la401</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RAEE01</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -193,7 +260,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -230,6 +297,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="27">
     <border>
@@ -553,7 +626,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -678,6 +751,12 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -998,17 +1077,18 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="AC4" sqref="AC4:AC9"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6:B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="5" customWidth="1"/>
+    <col min="1" max="1" width="6.25" customWidth="1"/>
     <col min="2" max="2" width="12.5" customWidth="1"/>
-    <col min="3" max="3" width="5" customWidth="1"/>
+    <col min="3" max="3" width="6.25" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
-    <col min="5" max="7" width="4.25" customWidth="1"/>
+    <col min="5" max="7" width="6.25" customWidth="1"/>
     <col min="8" max="20" width="4.375" customWidth="1"/>
+    <col min="21" max="21" width="6.375" customWidth="1"/>
     <col min="22" max="22" width="12.5" customWidth="1"/>
     <col min="23" max="25" width="4.25" customWidth="1"/>
     <col min="26" max="29" width="4.375" customWidth="1"/>
@@ -1022,7 +1102,7 @@
       </c>
       <c r="B1" s="5"/>
       <c r="C1" s="40" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="D1" s="37"/>
       <c r="E1" s="33" t="s">
@@ -1114,7 +1194,7 @@
       <c r="X2" s="14"/>
       <c r="Y2" s="15"/>
       <c r="Z2" s="13" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="AA2" s="14"/>
       <c r="AB2" s="14"/>
@@ -1203,22 +1283,22 @@
     </row>
     <row r="4" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A4" s="3">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C4" s="20">
         <v>0</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>30</v>
+        <v>22</v>
       </c>
       <c r="E4" s="20">
         <v>0</v>
       </c>
       <c r="F4" s="3">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G4" s="21">
         <v>0</v>
@@ -1263,9 +1343,11 @@
         <v>1</v>
       </c>
       <c r="U4" s="20">
-        <v>200</v>
-      </c>
-      <c r="V4" s="21"/>
+        <v>100</v>
+      </c>
+      <c r="V4" s="21" t="s">
+        <v>23</v>
+      </c>
       <c r="W4" s="20">
         <v>0</v>
       </c>
@@ -1276,10 +1358,10 @@
         <v>0</v>
       </c>
       <c r="Z4" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA4" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB4" s="3">
         <v>0</v>
@@ -1294,22 +1376,22 @@
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
-        <v>2</v>
+        <v>200</v>
       </c>
       <c r="B5" s="6" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C5" s="7">
-        <v>1</v>
+        <v>100</v>
       </c>
       <c r="D5" s="6" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="E5" s="7">
         <v>0</v>
       </c>
       <c r="F5" s="2">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G5" s="8">
         <v>0</v>
@@ -1356,7 +1438,9 @@
       <c r="U5" s="7">
         <v>200</v>
       </c>
-      <c r="V5" s="8"/>
+      <c r="V5" s="8" t="s">
+        <v>25</v>
+      </c>
       <c r="W5" s="7">
         <v>0</v>
       </c>
@@ -1367,10 +1451,10 @@
         <v>0</v>
       </c>
       <c r="Z5" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB5" s="3">
         <v>0</v>
@@ -1385,22 +1469,22 @@
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="B6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="20">
+        <v>200</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="20">
+      <c r="E6" s="20">
         <v>2</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="20">
-        <v>0</v>
-      </c>
       <c r="F6" s="3">
-        <v>3</v>
+        <v>10</v>
       </c>
       <c r="G6" s="21">
         <v>0</v>
@@ -1445,9 +1529,11 @@
         <v>1</v>
       </c>
       <c r="U6" s="7">
-        <v>200</v>
-      </c>
-      <c r="V6" s="8"/>
+        <v>300</v>
+      </c>
+      <c r="V6" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="W6" s="20">
         <v>0</v>
       </c>
@@ -1458,10 +1544,10 @@
         <v>0</v>
       </c>
       <c r="Z6" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA6" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB6" s="3">
         <v>0</v>
@@ -1476,22 +1562,22 @@
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
-        <v>4</v>
+        <v>301</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C7" s="7">
-        <v>3</v>
+        <v>300</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
       <c r="E7" s="7">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F7" s="2">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="G7" s="8">
         <v>0</v>
@@ -1536,9 +1622,11 @@
         <v>1</v>
       </c>
       <c r="U7" s="7">
-        <v>200</v>
-      </c>
-      <c r="V7" s="8"/>
+        <v>300</v>
+      </c>
+      <c r="V7" s="8" t="s">
+        <v>27</v>
+      </c>
       <c r="W7" s="7">
         <v>0</v>
       </c>
@@ -1549,10 +1637,10 @@
         <v>0</v>
       </c>
       <c r="Z7" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA7" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB7" s="3">
         <v>0</v>
@@ -1567,22 +1655,22 @@
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A8" s="2">
-        <v>5</v>
+        <v>302</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="C8" s="20">
-        <v>4</v>
+        <v>301</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>21</v>
+        <v>28</v>
       </c>
       <c r="E8" s="20">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="F8" s="3">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G8" s="21">
         <v>0</v>
@@ -1627,9 +1715,11 @@
         <v>1</v>
       </c>
       <c r="U8" s="7">
-        <v>200</v>
-      </c>
-      <c r="V8" s="8"/>
+        <v>301</v>
+      </c>
+      <c r="V8" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="W8" s="20">
         <v>0</v>
       </c>
@@ -1640,10 +1730,10 @@
         <v>0</v>
       </c>
       <c r="Z8" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA8" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB8" s="3">
         <v>0</v>
@@ -1658,22 +1748,22 @@
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
-        <v>6</v>
+        <v>400</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C9" s="7">
-        <v>5</v>
+        <v>100</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="E9" s="7">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F9" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G9" s="8">
         <v>0</v>
@@ -1718,23 +1808,25 @@
         <v>1</v>
       </c>
       <c r="U9" s="7">
-        <v>200</v>
-      </c>
-      <c r="V9" s="8"/>
-      <c r="W9" s="7">
-        <v>0</v>
-      </c>
-      <c r="X9" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y9" s="8">
+        <v>400</v>
+      </c>
+      <c r="V9" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W9" s="20">
+        <v>0</v>
+      </c>
+      <c r="X9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y9" s="21">
         <v>0</v>
       </c>
       <c r="Z9" s="20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AA9" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AB9" s="3">
         <v>0</v>
@@ -1748,519 +1840,1119 @@
       <c r="AE9" s="8"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A10" s="2"/>
-      <c r="B10" s="6"/>
-      <c r="C10" s="7"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="7"/>
-      <c r="F10" s="2"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="2"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="8"/>
-      <c r="L10" s="7"/>
-      <c r="M10" s="2"/>
-      <c r="N10" s="8"/>
-      <c r="O10" s="7"/>
-      <c r="P10" s="2"/>
-      <c r="Q10" s="8"/>
-      <c r="R10" s="7"/>
-      <c r="S10" s="2"/>
-      <c r="T10" s="8"/>
-      <c r="U10" s="7"/>
-      <c r="V10" s="8"/>
-      <c r="W10" s="7"/>
-      <c r="X10" s="2"/>
-      <c r="Y10" s="8"/>
-      <c r="Z10" s="7"/>
-      <c r="AA10" s="2"/>
-      <c r="AB10" s="2"/>
-      <c r="AC10" s="8"/>
-      <c r="AD10" s="8"/>
+      <c r="A10" s="2">
+        <v>401</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="7">
+        <v>400</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="E10" s="7">
+        <v>-2</v>
+      </c>
+      <c r="F10" s="2">
+        <v>8</v>
+      </c>
+      <c r="G10" s="8">
+        <v>0</v>
+      </c>
+      <c r="H10" s="20">
+        <v>0</v>
+      </c>
+      <c r="I10" s="3">
+        <v>1</v>
+      </c>
+      <c r="J10" s="3">
+        <v>0</v>
+      </c>
+      <c r="K10" s="21">
+        <v>0</v>
+      </c>
+      <c r="L10" s="20">
+        <v>1</v>
+      </c>
+      <c r="M10" s="3">
+        <v>0</v>
+      </c>
+      <c r="N10" s="21">
+        <v>0</v>
+      </c>
+      <c r="O10" s="20">
+        <v>0</v>
+      </c>
+      <c r="P10" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q10" s="21">
+        <v>0</v>
+      </c>
+      <c r="R10" s="20">
+        <v>0</v>
+      </c>
+      <c r="S10" s="3">
+        <v>0</v>
+      </c>
+      <c r="T10" s="21">
+        <v>1</v>
+      </c>
+      <c r="U10" s="7">
+        <v>400</v>
+      </c>
+      <c r="V10" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="W10" s="20">
+        <v>0</v>
+      </c>
+      <c r="X10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y10" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB10" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD10" s="8">
+        <v>1</v>
+      </c>
       <c r="AE10" s="8"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A11" s="2">
-        <v>100</v>
+        <v>402</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C11" s="7">
-        <v>6</v>
+        <v>401</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>32</v>
       </c>
       <c r="E11" s="7">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F11" s="2">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G11" s="8">
         <v>0</v>
       </c>
-      <c r="H11" s="7">
-        <v>0</v>
-      </c>
-      <c r="I11" s="2">
-        <v>1</v>
-      </c>
-      <c r="J11" s="2">
-        <v>0</v>
-      </c>
-      <c r="K11" s="8">
-        <v>0</v>
-      </c>
-      <c r="L11" s="7">
-        <v>1</v>
-      </c>
-      <c r="M11" s="2">
-        <v>0</v>
-      </c>
-      <c r="N11" s="8">
-        <v>0</v>
-      </c>
-      <c r="O11" s="7">
-        <v>0</v>
-      </c>
-      <c r="P11" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q11" s="8">
-        <v>0</v>
-      </c>
-      <c r="R11" s="7">
-        <v>0</v>
-      </c>
-      <c r="S11" s="2">
-        <v>0</v>
-      </c>
-      <c r="T11" s="8">
+      <c r="H11" s="20">
+        <v>0</v>
+      </c>
+      <c r="I11" s="3">
+        <v>1</v>
+      </c>
+      <c r="J11" s="3">
+        <v>0</v>
+      </c>
+      <c r="K11" s="21">
+        <v>0</v>
+      </c>
+      <c r="L11" s="20">
+        <v>1</v>
+      </c>
+      <c r="M11" s="3">
+        <v>0</v>
+      </c>
+      <c r="N11" s="21">
+        <v>0</v>
+      </c>
+      <c r="O11" s="20">
+        <v>0</v>
+      </c>
+      <c r="P11" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q11" s="21">
+        <v>0</v>
+      </c>
+      <c r="R11" s="20">
+        <v>0</v>
+      </c>
+      <c r="S11" s="3">
+        <v>0</v>
+      </c>
+      <c r="T11" s="21">
         <v>1</v>
       </c>
       <c r="U11" s="7">
-        <v>200</v>
-      </c>
-      <c r="V11" s="8"/>
-      <c r="W11" s="7">
-        <v>0</v>
-      </c>
-      <c r="X11" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y11" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA11" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB11" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC11" s="8">
+        <v>401</v>
+      </c>
+      <c r="V11" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="W11" s="20">
+        <v>0</v>
+      </c>
+      <c r="X11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y11" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB11" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="21">
         <v>0</v>
       </c>
       <c r="AD11" s="8">
         <v>1</v>
       </c>
-      <c r="AE11" s="8" t="s">
-        <v>33</v>
-      </c>
+      <c r="AE11" s="8"/>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A12" s="2"/>
-      <c r="B12" s="6"/>
-      <c r="C12" s="7"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="7"/>
-      <c r="F12" s="2"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="8"/>
-      <c r="L12" s="7"/>
-      <c r="M12" s="2"/>
-      <c r="N12" s="8"/>
-      <c r="O12" s="7"/>
-      <c r="P12" s="2"/>
-      <c r="Q12" s="8"/>
-      <c r="R12" s="7"/>
-      <c r="S12" s="2"/>
-      <c r="T12" s="8"/>
-      <c r="U12" s="7"/>
-      <c r="V12" s="8"/>
-      <c r="W12" s="7"/>
-      <c r="X12" s="2"/>
-      <c r="Y12" s="8"/>
-      <c r="Z12" s="7"/>
-      <c r="AA12" s="2"/>
-      <c r="AB12" s="2"/>
-      <c r="AC12" s="8"/>
-      <c r="AD12" s="8"/>
+      <c r="A12" s="2">
+        <v>500</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C12" s="7">
+        <v>100</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E12" s="7">
+        <v>0</v>
+      </c>
+      <c r="F12" s="2">
+        <v>10</v>
+      </c>
+      <c r="G12" s="8">
+        <v>0</v>
+      </c>
+      <c r="H12" s="20">
+        <v>0</v>
+      </c>
+      <c r="I12" s="3">
+        <v>1</v>
+      </c>
+      <c r="J12" s="3">
+        <v>0</v>
+      </c>
+      <c r="K12" s="21">
+        <v>0</v>
+      </c>
+      <c r="L12" s="20">
+        <v>1</v>
+      </c>
+      <c r="M12" s="3">
+        <v>0</v>
+      </c>
+      <c r="N12" s="21">
+        <v>0</v>
+      </c>
+      <c r="O12" s="20">
+        <v>0</v>
+      </c>
+      <c r="P12" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q12" s="21">
+        <v>0</v>
+      </c>
+      <c r="R12" s="20">
+        <v>0</v>
+      </c>
+      <c r="S12" s="3">
+        <v>0</v>
+      </c>
+      <c r="T12" s="21">
+        <v>1</v>
+      </c>
+      <c r="U12" s="7">
+        <v>500</v>
+      </c>
+      <c r="V12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="W12" s="20">
+        <v>0</v>
+      </c>
+      <c r="X12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y12" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB12" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD12" s="8">
+        <v>1</v>
+      </c>
       <c r="AE12" s="8"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
+        <v>501</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="7">
+        <v>500</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>10.75</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0</v>
+      </c>
+      <c r="H13" s="20">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="21">
+        <v>0</v>
+      </c>
+      <c r="L13" s="20">
+        <v>1</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0</v>
+      </c>
+      <c r="N13" s="21">
+        <v>0</v>
+      </c>
+      <c r="O13" s="20">
+        <v>0</v>
+      </c>
+      <c r="P13" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="21">
+        <v>0</v>
+      </c>
+      <c r="R13" s="20">
+        <v>0</v>
+      </c>
+      <c r="S13" s="3">
+        <v>0</v>
+      </c>
+      <c r="T13" s="21">
+        <v>1</v>
+      </c>
+      <c r="U13" s="7">
+        <v>501</v>
+      </c>
+      <c r="V13" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="W13" s="20">
+        <v>0</v>
+      </c>
+      <c r="X13" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y13" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB13" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD13" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE13" s="8"/>
+    </row>
+    <row r="14" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A14" s="2">
+        <v>600</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="7">
         <v>200</v>
       </c>
-      <c r="B13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C13" s="7">
-        <v>0</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="E13" s="7">
+      <c r="D14" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E14" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="F14" s="2">
+        <v>6</v>
+      </c>
+      <c r="G14" s="8">
+        <v>0</v>
+      </c>
+      <c r="H14" s="20">
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <v>1</v>
+      </c>
+      <c r="J14" s="3">
+        <v>0</v>
+      </c>
+      <c r="K14" s="21">
+        <v>0</v>
+      </c>
+      <c r="L14" s="20">
+        <v>1</v>
+      </c>
+      <c r="M14" s="3">
+        <v>0</v>
+      </c>
+      <c r="N14" s="21">
+        <v>0</v>
+      </c>
+      <c r="O14" s="20">
+        <v>0</v>
+      </c>
+      <c r="P14" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q14" s="21">
+        <v>0</v>
+      </c>
+      <c r="R14" s="20">
+        <v>0</v>
+      </c>
+      <c r="S14" s="3">
+        <v>0</v>
+      </c>
+      <c r="T14" s="21">
+        <v>1</v>
+      </c>
+      <c r="U14" s="7">
+        <v>600</v>
+      </c>
+      <c r="V14" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="W14" s="20">
+        <v>0</v>
+      </c>
+      <c r="X14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y14" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB14" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD14" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE14" s="8"/>
+    </row>
+    <row r="15" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A15" s="2">
+        <v>601</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="7">
+        <v>600</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="E15" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="F15" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="G15" s="8">
+        <v>0</v>
+      </c>
+      <c r="H15" s="20">
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <v>1</v>
+      </c>
+      <c r="J15" s="3">
+        <v>0</v>
+      </c>
+      <c r="K15" s="21">
+        <v>0</v>
+      </c>
+      <c r="L15" s="20">
+        <v>1</v>
+      </c>
+      <c r="M15" s="3">
+        <v>0</v>
+      </c>
+      <c r="N15" s="21">
+        <v>0</v>
+      </c>
+      <c r="O15" s="20">
+        <v>0</v>
+      </c>
+      <c r="P15" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q15" s="21">
+        <v>0</v>
+      </c>
+      <c r="R15" s="20">
+        <v>0</v>
+      </c>
+      <c r="S15" s="3">
+        <v>0</v>
+      </c>
+      <c r="T15" s="21">
+        <v>1</v>
+      </c>
+      <c r="U15" s="7">
+        <v>600</v>
+      </c>
+      <c r="V15" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="W15" s="20">
+        <v>0</v>
+      </c>
+      <c r="X15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y15" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB15" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD15" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE15" s="8"/>
+    </row>
+    <row r="16" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A16" s="2">
+        <v>602</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="7">
+        <v>601</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E16" s="7">
+        <v>1.5</v>
+      </c>
+      <c r="F16" s="2">
+        <v>1</v>
+      </c>
+      <c r="G16" s="8">
+        <v>0</v>
+      </c>
+      <c r="H16" s="20">
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <v>1</v>
+      </c>
+      <c r="J16" s="3">
+        <v>0</v>
+      </c>
+      <c r="K16" s="21">
+        <v>0</v>
+      </c>
+      <c r="L16" s="20">
+        <v>1</v>
+      </c>
+      <c r="M16" s="3">
+        <v>0</v>
+      </c>
+      <c r="N16" s="21">
+        <v>0</v>
+      </c>
+      <c r="O16" s="20">
+        <v>0</v>
+      </c>
+      <c r="P16" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q16" s="21">
+        <v>0</v>
+      </c>
+      <c r="R16" s="20">
+        <v>0</v>
+      </c>
+      <c r="S16" s="3">
+        <v>0</v>
+      </c>
+      <c r="T16" s="21">
+        <v>1</v>
+      </c>
+      <c r="U16" s="7">
+        <v>601</v>
+      </c>
+      <c r="V16" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="W16" s="20">
+        <v>0</v>
+      </c>
+      <c r="X16" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y16" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB16" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD16" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE16" s="8"/>
+    </row>
+    <row r="17" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A17" s="2">
+        <v>700</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C17" s="7">
+        <v>200</v>
+      </c>
+      <c r="D17" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E17" s="7">
+        <v>-1.5</v>
+      </c>
+      <c r="F17" s="2">
+        <v>6</v>
+      </c>
+      <c r="G17" s="8">
+        <v>0</v>
+      </c>
+      <c r="H17" s="20">
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <v>1</v>
+      </c>
+      <c r="J17" s="3">
+        <v>0</v>
+      </c>
+      <c r="K17" s="21">
+        <v>0</v>
+      </c>
+      <c r="L17" s="20">
+        <v>1</v>
+      </c>
+      <c r="M17" s="3">
+        <v>0</v>
+      </c>
+      <c r="N17" s="21">
+        <v>0</v>
+      </c>
+      <c r="O17" s="20">
+        <v>0</v>
+      </c>
+      <c r="P17" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q17" s="21">
+        <v>0</v>
+      </c>
+      <c r="R17" s="20">
+        <v>0</v>
+      </c>
+      <c r="S17" s="3">
+        <v>0</v>
+      </c>
+      <c r="T17" s="21">
+        <v>1</v>
+      </c>
+      <c r="U17" s="7">
+        <v>700</v>
+      </c>
+      <c r="V17" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="W17" s="20">
+        <v>0</v>
+      </c>
+      <c r="X17" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y17" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB17" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD17" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE17" s="8"/>
+    </row>
+    <row r="18" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A18" s="2">
+        <v>701</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="7">
+        <v>700</v>
+      </c>
+      <c r="D18" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E18" s="7">
+        <v>-1.5</v>
+      </c>
+      <c r="F18" s="2">
+        <v>3.5</v>
+      </c>
+      <c r="G18" s="8">
+        <v>0</v>
+      </c>
+      <c r="H18" s="20">
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <v>1</v>
+      </c>
+      <c r="J18" s="3">
+        <v>0</v>
+      </c>
+      <c r="K18" s="21">
+        <v>0</v>
+      </c>
+      <c r="L18" s="20">
+        <v>1</v>
+      </c>
+      <c r="M18" s="3">
+        <v>0</v>
+      </c>
+      <c r="N18" s="21">
+        <v>0</v>
+      </c>
+      <c r="O18" s="20">
+        <v>0</v>
+      </c>
+      <c r="P18" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q18" s="21">
+        <v>0</v>
+      </c>
+      <c r="R18" s="20">
+        <v>0</v>
+      </c>
+      <c r="S18" s="3">
+        <v>0</v>
+      </c>
+      <c r="T18" s="21">
+        <v>1</v>
+      </c>
+      <c r="U18" s="7">
+        <v>700</v>
+      </c>
+      <c r="V18" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="W18" s="20">
+        <v>0</v>
+      </c>
+      <c r="X18" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y18" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB18" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD18" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE18" s="8"/>
+    </row>
+    <row r="19" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A19" s="2">
+        <v>702</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="7">
+        <v>701</v>
+      </c>
+      <c r="D19" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E19" s="7">
+        <v>-1.5</v>
+      </c>
+      <c r="F19" s="2">
+        <v>1</v>
+      </c>
+      <c r="G19" s="8">
+        <v>0</v>
+      </c>
+      <c r="H19" s="20">
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <v>1</v>
+      </c>
+      <c r="J19" s="3">
+        <v>0</v>
+      </c>
+      <c r="K19" s="21">
+        <v>0</v>
+      </c>
+      <c r="L19" s="20">
+        <v>1</v>
+      </c>
+      <c r="M19" s="3">
+        <v>0</v>
+      </c>
+      <c r="N19" s="21">
+        <v>0</v>
+      </c>
+      <c r="O19" s="20">
+        <v>0</v>
+      </c>
+      <c r="P19" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q19" s="21">
+        <v>0</v>
+      </c>
+      <c r="R19" s="20">
+        <v>0</v>
+      </c>
+      <c r="S19" s="3">
+        <v>0</v>
+      </c>
+      <c r="T19" s="21">
+        <v>1</v>
+      </c>
+      <c r="U19" s="7">
+        <v>701</v>
+      </c>
+      <c r="V19" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="W19" s="20">
+        <v>0</v>
+      </c>
+      <c r="X19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE19" s="8"/>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A20" s="2">
+        <v>1300</v>
+      </c>
+      <c r="B20" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C20" s="7">
+        <v>302</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E20" s="7">
+        <v>2</v>
+      </c>
+      <c r="F20" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+      <c r="H20" s="20">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0</v>
+      </c>
+      <c r="K20" s="21">
+        <v>0</v>
+      </c>
+      <c r="L20" s="20">
+        <v>1</v>
+      </c>
+      <c r="M20" s="3">
+        <v>0</v>
+      </c>
+      <c r="N20" s="21">
+        <v>0</v>
+      </c>
+      <c r="O20" s="20">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="21">
+        <v>0</v>
+      </c>
+      <c r="R20" s="20">
+        <v>0</v>
+      </c>
+      <c r="S20" s="3">
+        <v>0</v>
+      </c>
+      <c r="T20" s="21">
+        <v>1</v>
+      </c>
+      <c r="U20" s="7">
+        <v>0</v>
+      </c>
+      <c r="V20" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="W20" s="20">
+        <v>0</v>
+      </c>
+      <c r="X20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE20" s="8"/>
+    </row>
+    <row r="21" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A21" s="2">
+        <v>2300</v>
+      </c>
+      <c r="B21" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C21" s="7">
+        <v>0</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E21" s="7">
         <v>3</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F21" s="2">
+        <v>8</v>
+      </c>
+      <c r="G21" s="8">
         <v>3</v>
       </c>
-      <c r="G13" s="8">
-        <v>3</v>
-      </c>
-      <c r="H13" s="7">
-        <v>0</v>
-      </c>
-      <c r="I13" s="2">
-        <v>1</v>
-      </c>
-      <c r="J13" s="2">
-        <v>0</v>
-      </c>
-      <c r="K13" s="8">
-        <v>0</v>
-      </c>
-      <c r="L13" s="7">
-        <v>1</v>
-      </c>
-      <c r="M13" s="2">
-        <v>0</v>
-      </c>
-      <c r="N13" s="8">
-        <v>0</v>
-      </c>
-      <c r="O13" s="7">
-        <v>0</v>
-      </c>
-      <c r="P13" s="2">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="8">
-        <v>0</v>
-      </c>
-      <c r="R13" s="7">
-        <v>0</v>
-      </c>
-      <c r="S13" s="2">
-        <v>0</v>
-      </c>
-      <c r="T13" s="8">
-        <v>1</v>
-      </c>
-      <c r="U13" s="7">
-        <v>200</v>
-      </c>
-      <c r="V13" s="8"/>
-      <c r="W13" s="7">
-        <v>0</v>
-      </c>
-      <c r="X13" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y13" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="7">
-        <v>1</v>
-      </c>
-      <c r="AA13" s="2">
-        <v>0</v>
-      </c>
-      <c r="AB13" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC13" s="8">
-        <v>0</v>
-      </c>
-      <c r="AD13" s="8">
-        <v>1</v>
-      </c>
-      <c r="AE13" s="8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A14" s="2"/>
-      <c r="B14" s="6"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="8"/>
-      <c r="L14" s="7"/>
-      <c r="M14" s="2"/>
-      <c r="N14" s="8"/>
-      <c r="O14" s="7"/>
-      <c r="P14" s="2"/>
-      <c r="Q14" s="8"/>
-      <c r="R14" s="7"/>
-      <c r="S14" s="2"/>
-      <c r="T14" s="8"/>
-      <c r="U14" s="7"/>
-      <c r="V14" s="8"/>
-      <c r="W14" s="7"/>
-      <c r="X14" s="2"/>
-      <c r="Y14" s="8"/>
-      <c r="Z14" s="7"/>
-      <c r="AA14" s="2"/>
-      <c r="AB14" s="2"/>
-      <c r="AC14" s="8"/>
-      <c r="AD14" s="8"/>
-      <c r="AE14" s="8"/>
-    </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A15" s="2"/>
-      <c r="B15" s="6"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="6"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="7"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="7"/>
-      <c r="M15" s="2"/>
-      <c r="N15" s="8"/>
-      <c r="O15" s="7"/>
-      <c r="P15" s="2"/>
-      <c r="Q15" s="8"/>
-      <c r="R15" s="7"/>
-      <c r="S15" s="2"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="7"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="7"/>
-      <c r="X15" s="2"/>
-      <c r="Y15" s="8"/>
-      <c r="Z15" s="7"/>
-      <c r="AA15" s="2"/>
-      <c r="AB15" s="2"/>
-      <c r="AC15" s="8"/>
-      <c r="AD15" s="8"/>
-      <c r="AE15" s="8"/>
-    </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A16" s="2"/>
-      <c r="B16" s="6"/>
-      <c r="C16" s="7"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="7"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="2"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="8"/>
-      <c r="L16" s="7"/>
-      <c r="M16" s="2"/>
-      <c r="N16" s="8"/>
-      <c r="O16" s="7"/>
-      <c r="P16" s="2"/>
-      <c r="Q16" s="8"/>
-      <c r="R16" s="7"/>
-      <c r="S16" s="2"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="7"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="7"/>
-      <c r="X16" s="2"/>
-      <c r="Y16" s="8"/>
-      <c r="Z16" s="7"/>
-      <c r="AA16" s="2"/>
-      <c r="AB16" s="2"/>
-      <c r="AC16" s="8"/>
-      <c r="AD16" s="8"/>
-      <c r="AE16" s="8"/>
-    </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A17" s="2"/>
-      <c r="B17" s="6"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="7"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="2"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="8"/>
-      <c r="L17" s="7"/>
-      <c r="M17" s="2"/>
-      <c r="N17" s="8"/>
-      <c r="O17" s="7"/>
-      <c r="P17" s="2"/>
-      <c r="Q17" s="8"/>
-      <c r="R17" s="7"/>
-      <c r="S17" s="2"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="7"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="7"/>
-      <c r="X17" s="2"/>
-      <c r="Y17" s="8"/>
-      <c r="Z17" s="7"/>
-      <c r="AA17" s="2"/>
-      <c r="AB17" s="2"/>
-      <c r="AC17" s="8"/>
-      <c r="AD17" s="8"/>
-      <c r="AE17" s="8"/>
-    </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A18" s="2"/>
-      <c r="B18" s="6"/>
-      <c r="C18" s="7"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="2"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="2"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="8"/>
-      <c r="L18" s="7"/>
-      <c r="M18" s="2"/>
-      <c r="N18" s="8"/>
-      <c r="O18" s="7"/>
-      <c r="P18" s="2"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="7"/>
-      <c r="S18" s="2"/>
-      <c r="T18" s="8"/>
-      <c r="U18" s="7"/>
-      <c r="V18" s="8"/>
-      <c r="W18" s="7"/>
-      <c r="X18" s="2"/>
-      <c r="Y18" s="8"/>
-      <c r="Z18" s="7"/>
-      <c r="AA18" s="2"/>
-      <c r="AB18" s="2"/>
-      <c r="AC18" s="8"/>
-      <c r="AD18" s="8"/>
-      <c r="AE18" s="8"/>
-    </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A19" s="2"/>
-      <c r="B19" s="6"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="6"/>
-      <c r="E19" s="7"/>
-      <c r="F19" s="2"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="2"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="8"/>
-      <c r="L19" s="7"/>
-      <c r="M19" s="2"/>
-      <c r="N19" s="8"/>
-      <c r="O19" s="7"/>
-      <c r="P19" s="2"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="7"/>
-      <c r="S19" s="2"/>
-      <c r="T19" s="8"/>
-      <c r="U19" s="7"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="7"/>
-      <c r="X19" s="2"/>
-      <c r="Y19" s="8"/>
-      <c r="Z19" s="7"/>
-      <c r="AA19" s="2"/>
-      <c r="AB19" s="2"/>
-      <c r="AC19" s="8"/>
-      <c r="AD19" s="8"/>
-      <c r="AE19" s="8"/>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A20" s="2"/>
-      <c r="B20" s="6"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="2"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="8"/>
-      <c r="L20" s="7"/>
-      <c r="M20" s="2"/>
-      <c r="N20" s="8"/>
-      <c r="O20" s="7"/>
-      <c r="P20" s="2"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="7"/>
-      <c r="S20" s="2"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="7"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="7"/>
-      <c r="X20" s="2"/>
-      <c r="Y20" s="8"/>
-      <c r="Z20" s="7"/>
-      <c r="AA20" s="2"/>
-      <c r="AB20" s="2"/>
-      <c r="AC20" s="8"/>
-      <c r="AD20" s="8"/>
-      <c r="AE20" s="8"/>
-    </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A21" s="2"/>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="6"/>
-      <c r="E21" s="7"/>
-      <c r="F21" s="2"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="7"/>
-      <c r="I21" s="2"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="8"/>
-      <c r="L21" s="7"/>
-      <c r="M21" s="2"/>
-      <c r="N21" s="8"/>
-      <c r="O21" s="7"/>
-      <c r="P21" s="2"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="7"/>
-      <c r="S21" s="2"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="7"/>
-      <c r="V21" s="8"/>
-      <c r="W21" s="7"/>
-      <c r="X21" s="2"/>
-      <c r="Y21" s="8"/>
-      <c r="Z21" s="7"/>
-      <c r="AA21" s="2"/>
-      <c r="AB21" s="2"/>
-      <c r="AC21" s="8"/>
-      <c r="AD21" s="8"/>
+      <c r="H21" s="20">
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <v>1</v>
+      </c>
+      <c r="J21" s="3">
+        <v>0</v>
+      </c>
+      <c r="K21" s="21">
+        <v>0</v>
+      </c>
+      <c r="L21" s="20">
+        <v>1</v>
+      </c>
+      <c r="M21" s="3">
+        <v>0</v>
+      </c>
+      <c r="N21" s="21">
+        <v>0</v>
+      </c>
+      <c r="O21" s="20">
+        <v>0</v>
+      </c>
+      <c r="P21" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q21" s="21">
+        <v>0</v>
+      </c>
+      <c r="R21" s="20">
+        <v>0</v>
+      </c>
+      <c r="S21" s="3">
+        <v>0</v>
+      </c>
+      <c r="T21" s="21">
+        <v>1</v>
+      </c>
+      <c r="U21" s="7">
+        <v>0</v>
+      </c>
+      <c r="V21" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="W21" s="20">
+        <v>0</v>
+      </c>
+      <c r="X21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y21" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB21" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD21" s="8">
+        <v>1</v>
+      </c>
       <c r="AE21" s="8"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
debug : [TPSCameraDirector] : forcus_point update.
</commit_message>
<xml_diff>
--- a/gameCSV/Actor_RobotObj_01.xlsx
+++ b/gameCSV/Actor_RobotObj_01.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltz\Documents\CppProjects\GitManagements\QuantumCoreRobotReMake\gameCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{104B69C7-339F-4A8C-A822-2F0B79754EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D790327-7776-4AFF-A833-4A26CA8E86C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16800" yWindow="2445" windowWidth="17160" windowHeight="10980" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
   </bookViews>
   <sheets>
     <sheet name="Actor_RobotObj_01" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
   <si>
     <t>id</t>
     <phoneticPr fontId="1"/>
@@ -236,6 +236,62 @@
   </si>
   <si>
     <t>RAEE01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Right Wrist Obj</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Right Wrist Tar</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RAEE02</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RATA02</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Lower Body</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Body</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Rright Arm</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Left Arm</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Head</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Right Leg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Left Leg</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Right elbow Obj</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Right elbow Tar</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>non</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -626,7 +682,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -757,6 +813,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1077,7 +1136,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6:B8"/>
+      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1372,7 +1431,9 @@
       <c r="AD4" s="21">
         <v>1</v>
       </c>
-      <c r="AE4" s="21"/>
+      <c r="AE4" s="21" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A5" s="2">
@@ -1465,7 +1526,9 @@
       <c r="AD5" s="21">
         <v>1</v>
       </c>
-      <c r="AE5" s="8"/>
+      <c r="AE5" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
@@ -1558,7 +1621,9 @@
       <c r="AD6" s="21">
         <v>1</v>
       </c>
-      <c r="AE6" s="8"/>
+      <c r="AE6" s="8" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
@@ -1837,7 +1902,9 @@
       <c r="AD9" s="8">
         <v>1</v>
       </c>
-      <c r="AE9" s="8"/>
+      <c r="AE9" s="8" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A10" s="2">
@@ -2116,7 +2183,9 @@
       <c r="AD12" s="8">
         <v>1</v>
       </c>
-      <c r="AE12" s="8"/>
+      <c r="AE12" s="8" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
@@ -2302,7 +2371,9 @@
       <c r="AD14" s="8">
         <v>1</v>
       </c>
-      <c r="AE14" s="8"/>
+      <c r="AE14" s="8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A15" s="2">
@@ -2581,7 +2652,9 @@
       <c r="AD17" s="8">
         <v>1</v>
       </c>
-      <c r="AE17" s="8"/>
+      <c r="AE17" s="8" t="s">
+        <v>63</v>
+      </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A18" s="2">
@@ -2770,212 +2843,92 @@
       <c r="AE19" s="8"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A20" s="2">
-        <v>1300</v>
-      </c>
-      <c r="B20" s="42" t="s">
-        <v>52</v>
-      </c>
-      <c r="C20" s="7">
-        <v>302</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E20" s="7">
-        <v>2</v>
-      </c>
-      <c r="F20" s="2">
-        <v>5.5</v>
-      </c>
-      <c r="G20" s="8">
-        <v>0</v>
-      </c>
-      <c r="H20" s="20">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3">
-        <v>1</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0</v>
-      </c>
-      <c r="K20" s="21">
-        <v>0</v>
-      </c>
-      <c r="L20" s="20">
-        <v>1</v>
-      </c>
-      <c r="M20" s="3">
-        <v>0</v>
-      </c>
-      <c r="N20" s="21">
-        <v>0</v>
-      </c>
-      <c r="O20" s="20">
-        <v>0</v>
-      </c>
-      <c r="P20" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="21">
-        <v>0</v>
-      </c>
-      <c r="R20" s="20">
-        <v>0</v>
-      </c>
-      <c r="S20" s="3">
-        <v>0</v>
-      </c>
-      <c r="T20" s="21">
-        <v>1</v>
-      </c>
-      <c r="U20" s="7">
-        <v>0</v>
-      </c>
-      <c r="V20" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="W20" s="20">
-        <v>0</v>
-      </c>
-      <c r="X20" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="3">
-        <v>1</v>
-      </c>
-      <c r="AB20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="21">
-        <v>0</v>
-      </c>
-      <c r="AD20" s="8">
-        <v>1</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="20"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="21"/>
+      <c r="Z20" s="20"/>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3"/>
+      <c r="AC20" s="21"/>
+      <c r="AD20" s="8"/>
       <c r="AE20" s="8"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A21" s="2">
-        <v>2300</v>
-      </c>
-      <c r="B21" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" s="7">
-        <v>0</v>
-      </c>
-      <c r="D21" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="E21" s="7">
-        <v>3</v>
-      </c>
-      <c r="F21" s="2">
-        <v>8</v>
-      </c>
-      <c r="G21" s="8">
-        <v>3</v>
-      </c>
-      <c r="H21" s="20">
-        <v>0</v>
-      </c>
-      <c r="I21" s="3">
-        <v>1</v>
-      </c>
-      <c r="J21" s="3">
-        <v>0</v>
-      </c>
-      <c r="K21" s="21">
-        <v>0</v>
-      </c>
-      <c r="L21" s="20">
-        <v>1</v>
-      </c>
-      <c r="M21" s="3">
-        <v>0</v>
-      </c>
-      <c r="N21" s="21">
-        <v>0</v>
-      </c>
-      <c r="O21" s="20">
-        <v>0</v>
-      </c>
-      <c r="P21" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q21" s="21">
-        <v>0</v>
-      </c>
-      <c r="R21" s="20">
-        <v>0</v>
-      </c>
-      <c r="S21" s="3">
-        <v>0</v>
-      </c>
-      <c r="T21" s="21">
-        <v>1</v>
-      </c>
-      <c r="U21" s="7">
-        <v>0</v>
-      </c>
-      <c r="V21" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="W21" s="20">
-        <v>0</v>
-      </c>
-      <c r="X21" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y21" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA21" s="3">
-        <v>1</v>
-      </c>
-      <c r="AB21" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC21" s="21">
-        <v>0</v>
-      </c>
-      <c r="AD21" s="8">
-        <v>1</v>
-      </c>
+      <c r="A21" s="2"/>
+      <c r="B21" s="44"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="20"/>
+      <c r="I21" s="3"/>
+      <c r="J21" s="3"/>
+      <c r="K21" s="21"/>
+      <c r="L21" s="20"/>
+      <c r="M21" s="3"/>
+      <c r="N21" s="21"/>
+      <c r="O21" s="20"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="21"/>
+      <c r="R21" s="20"/>
+      <c r="S21" s="3"/>
+      <c r="T21" s="21"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="8"/>
+      <c r="W21" s="20"/>
+      <c r="X21" s="3"/>
+      <c r="Y21" s="21"/>
+      <c r="Z21" s="20"/>
+      <c r="AA21" s="3"/>
+      <c r="AB21" s="3"/>
+      <c r="AC21" s="21"/>
+      <c r="AD21" s="8"/>
       <c r="AE21" s="8"/>
     </row>
     <row r="22" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A22" s="2"/>
-      <c r="B22" s="6"/>
+      <c r="B22" s="44"/>
       <c r="C22" s="7"/>
       <c r="D22" s="6"/>
       <c r="E22" s="7"/>
       <c r="F22" s="2"/>
       <c r="G22" s="8"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="8"/>
-      <c r="L22" s="7"/>
-      <c r="M22" s="2"/>
-      <c r="N22" s="8"/>
-      <c r="O22" s="7"/>
-      <c r="P22" s="2"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="7"/>
-      <c r="S22" s="2"/>
-      <c r="T22" s="8"/>
+      <c r="H22" s="20"/>
+      <c r="I22" s="3"/>
+      <c r="J22" s="3"/>
+      <c r="K22" s="21"/>
+      <c r="L22" s="20"/>
+      <c r="M22" s="3"/>
+      <c r="N22" s="21"/>
+      <c r="O22" s="20"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="21"/>
+      <c r="R22" s="20"/>
+      <c r="S22" s="3"/>
+      <c r="T22" s="21"/>
       <c r="U22" s="7"/>
       <c r="V22" s="8"/>
       <c r="W22" s="7"/>
@@ -2990,25 +2943,25 @@
     </row>
     <row r="23" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A23" s="2"/>
-      <c r="B23" s="6"/>
+      <c r="B23" s="44"/>
       <c r="C23" s="7"/>
       <c r="D23" s="6"/>
       <c r="E23" s="7"/>
       <c r="F23" s="2"/>
       <c r="G23" s="8"/>
-      <c r="H23" s="7"/>
-      <c r="I23" s="2"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="8"/>
-      <c r="L23" s="7"/>
-      <c r="M23" s="2"/>
-      <c r="N23" s="8"/>
-      <c r="O23" s="7"/>
-      <c r="P23" s="2"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="7"/>
-      <c r="S23" s="2"/>
-      <c r="T23" s="8"/>
+      <c r="H23" s="20"/>
+      <c r="I23" s="3"/>
+      <c r="J23" s="3"/>
+      <c r="K23" s="21"/>
+      <c r="L23" s="20"/>
+      <c r="M23" s="3"/>
+      <c r="N23" s="21"/>
+      <c r="O23" s="20"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="21"/>
+      <c r="R23" s="20"/>
+      <c r="S23" s="3"/>
+      <c r="T23" s="21"/>
       <c r="U23" s="7"/>
       <c r="V23" s="8"/>
       <c r="W23" s="7"/>
@@ -3319,136 +3272,384 @@
       <c r="AE32" s="8"/>
     </row>
     <row r="33" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A33" s="2"/>
-      <c r="B33" s="6"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="6"/>
-      <c r="E33" s="7"/>
-      <c r="F33" s="2"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="7"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="2"/>
-      <c r="K33" s="8"/>
-      <c r="L33" s="7"/>
-      <c r="M33" s="2"/>
-      <c r="N33" s="8"/>
-      <c r="O33" s="7"/>
-      <c r="P33" s="2"/>
-      <c r="Q33" s="8"/>
-      <c r="R33" s="7"/>
-      <c r="S33" s="2"/>
-      <c r="T33" s="8"/>
-      <c r="U33" s="7"/>
-      <c r="V33" s="8"/>
-      <c r="W33" s="7"/>
-      <c r="X33" s="2"/>
-      <c r="Y33" s="8"/>
-      <c r="Z33" s="7"/>
-      <c r="AA33" s="2"/>
-      <c r="AB33" s="2"/>
-      <c r="AC33" s="8"/>
-      <c r="AD33" s="8"/>
-      <c r="AE33" s="8"/>
+      <c r="A33" s="2">
+        <v>1300</v>
+      </c>
+      <c r="B33" s="42" t="s">
+        <v>52</v>
+      </c>
+      <c r="C33" s="7">
+        <v>302</v>
+      </c>
+      <c r="D33" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="7">
+        <v>2</v>
+      </c>
+      <c r="F33" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="G33" s="8">
+        <v>0</v>
+      </c>
+      <c r="H33" s="20">
+        <v>0</v>
+      </c>
+      <c r="I33" s="3">
+        <v>1</v>
+      </c>
+      <c r="J33" s="3">
+        <v>0</v>
+      </c>
+      <c r="K33" s="21">
+        <v>0</v>
+      </c>
+      <c r="L33" s="20">
+        <v>1</v>
+      </c>
+      <c r="M33" s="3">
+        <v>0</v>
+      </c>
+      <c r="N33" s="21">
+        <v>0</v>
+      </c>
+      <c r="O33" s="20">
+        <v>0</v>
+      </c>
+      <c r="P33" s="3">
+        <v>-1</v>
+      </c>
+      <c r="Q33" s="21">
+        <v>0</v>
+      </c>
+      <c r="R33" s="20">
+        <v>0</v>
+      </c>
+      <c r="S33" s="3">
+        <v>0</v>
+      </c>
+      <c r="T33" s="21">
+        <v>-1</v>
+      </c>
+      <c r="U33" s="7">
+        <v>0</v>
+      </c>
+      <c r="V33" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="W33" s="20">
+        <v>0</v>
+      </c>
+      <c r="X33" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y33" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z33" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB33" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD33" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE33" s="8" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A34" s="2"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="6"/>
-      <c r="E34" s="7"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="8"/>
-      <c r="H34" s="7"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="2"/>
-      <c r="K34" s="8"/>
-      <c r="L34" s="7"/>
-      <c r="M34" s="2"/>
-      <c r="N34" s="8"/>
-      <c r="O34" s="7"/>
-      <c r="P34" s="2"/>
-      <c r="Q34" s="8"/>
-      <c r="R34" s="7"/>
-      <c r="S34" s="2"/>
-      <c r="T34" s="8"/>
-      <c r="U34" s="7"/>
-      <c r="V34" s="8"/>
-      <c r="W34" s="7"/>
-      <c r="X34" s="2"/>
-      <c r="Y34" s="8"/>
-      <c r="Z34" s="7"/>
-      <c r="AA34" s="2"/>
-      <c r="AB34" s="2"/>
-      <c r="AC34" s="8"/>
-      <c r="AD34" s="8"/>
-      <c r="AE34" s="8"/>
+      <c r="A34" s="2">
+        <v>2300</v>
+      </c>
+      <c r="B34" s="43" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="7">
+        <v>0</v>
+      </c>
+      <c r="D34" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E34" s="7">
+        <v>3</v>
+      </c>
+      <c r="F34" s="2">
+        <v>8</v>
+      </c>
+      <c r="G34" s="8">
+        <v>3</v>
+      </c>
+      <c r="H34" s="20">
+        <v>0</v>
+      </c>
+      <c r="I34" s="3">
+        <v>1</v>
+      </c>
+      <c r="J34" s="3">
+        <v>0</v>
+      </c>
+      <c r="K34" s="21">
+        <v>0</v>
+      </c>
+      <c r="L34" s="20">
+        <v>1</v>
+      </c>
+      <c r="M34" s="3">
+        <v>0</v>
+      </c>
+      <c r="N34" s="21">
+        <v>0</v>
+      </c>
+      <c r="O34" s="20">
+        <v>0</v>
+      </c>
+      <c r="P34" s="3">
+        <v>-1</v>
+      </c>
+      <c r="Q34" s="21">
+        <v>0</v>
+      </c>
+      <c r="R34" s="20">
+        <v>0</v>
+      </c>
+      <c r="S34" s="3">
+        <v>0</v>
+      </c>
+      <c r="T34" s="21">
+        <v>-1</v>
+      </c>
+      <c r="U34" s="7">
+        <v>0</v>
+      </c>
+      <c r="V34" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="W34" s="20">
+        <v>0</v>
+      </c>
+      <c r="X34" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y34" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z34" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB34" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD34" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE34" s="8" t="s">
+        <v>54</v>
+      </c>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A35" s="2"/>
-      <c r="B35" s="6"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="7"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="8"/>
-      <c r="H35" s="7"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="2"/>
-      <c r="K35" s="8"/>
-      <c r="L35" s="7"/>
-      <c r="M35" s="2"/>
-      <c r="N35" s="8"/>
-      <c r="O35" s="7"/>
-      <c r="P35" s="2"/>
-      <c r="Q35" s="8"/>
-      <c r="R35" s="7"/>
-      <c r="S35" s="2"/>
-      <c r="T35" s="8"/>
-      <c r="U35" s="7"/>
-      <c r="V35" s="8"/>
-      <c r="W35" s="7"/>
-      <c r="X35" s="2"/>
-      <c r="Y35" s="8"/>
-      <c r="Z35" s="7"/>
-      <c r="AA35" s="2"/>
-      <c r="AB35" s="2"/>
-      <c r="AC35" s="8"/>
-      <c r="AD35" s="8"/>
-      <c r="AE35" s="8"/>
+      <c r="A35" s="2">
+        <v>1301</v>
+      </c>
+      <c r="B35" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="C35" s="7">
+        <v>300</v>
+      </c>
+      <c r="D35" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="E35" s="7">
+        <v>2</v>
+      </c>
+      <c r="F35" s="2">
+        <v>8</v>
+      </c>
+      <c r="G35" s="8">
+        <v>0</v>
+      </c>
+      <c r="H35" s="20">
+        <v>0</v>
+      </c>
+      <c r="I35" s="3">
+        <v>1</v>
+      </c>
+      <c r="J35" s="3">
+        <v>0</v>
+      </c>
+      <c r="K35" s="21">
+        <v>0</v>
+      </c>
+      <c r="L35" s="20">
+        <v>1</v>
+      </c>
+      <c r="M35" s="3">
+        <v>0</v>
+      </c>
+      <c r="N35" s="21">
+        <v>0</v>
+      </c>
+      <c r="O35" s="20">
+        <v>0</v>
+      </c>
+      <c r="P35" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q35" s="21">
+        <v>0</v>
+      </c>
+      <c r="R35" s="20">
+        <v>0</v>
+      </c>
+      <c r="S35" s="3">
+        <v>0</v>
+      </c>
+      <c r="T35" s="21">
+        <v>1</v>
+      </c>
+      <c r="U35" s="7">
+        <v>0</v>
+      </c>
+      <c r="V35" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="W35" s="7">
+        <v>0</v>
+      </c>
+      <c r="X35" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y35" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB35" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD35" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE35" s="8" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A36" s="2"/>
-      <c r="B36" s="6"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="7"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="8"/>
-      <c r="H36" s="7"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="2"/>
-      <c r="K36" s="8"/>
-      <c r="L36" s="7"/>
-      <c r="M36" s="2"/>
-      <c r="N36" s="8"/>
-      <c r="O36" s="7"/>
-      <c r="P36" s="2"/>
-      <c r="Q36" s="8"/>
-      <c r="R36" s="7"/>
-      <c r="S36" s="2"/>
-      <c r="T36" s="8"/>
-      <c r="U36" s="7"/>
-      <c r="V36" s="8"/>
-      <c r="W36" s="7"/>
-      <c r="X36" s="2"/>
-      <c r="Y36" s="8"/>
-      <c r="Z36" s="7"/>
-      <c r="AA36" s="2"/>
-      <c r="AB36" s="2"/>
-      <c r="AC36" s="8"/>
-      <c r="AD36" s="8"/>
-      <c r="AE36" s="8"/>
+      <c r="A36" s="2">
+        <v>2301</v>
+      </c>
+      <c r="B36" s="43" t="s">
+        <v>56</v>
+      </c>
+      <c r="C36" s="7">
+        <v>200</v>
+      </c>
+      <c r="D36" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="7">
+        <v>3</v>
+      </c>
+      <c r="F36" s="2">
+        <v>8</v>
+      </c>
+      <c r="G36" s="8">
+        <v>0</v>
+      </c>
+      <c r="H36" s="20">
+        <v>0</v>
+      </c>
+      <c r="I36" s="3">
+        <v>1</v>
+      </c>
+      <c r="J36" s="3">
+        <v>0</v>
+      </c>
+      <c r="K36" s="21">
+        <v>0</v>
+      </c>
+      <c r="L36" s="20">
+        <v>1</v>
+      </c>
+      <c r="M36" s="3">
+        <v>0</v>
+      </c>
+      <c r="N36" s="21">
+        <v>0</v>
+      </c>
+      <c r="O36" s="20">
+        <v>0</v>
+      </c>
+      <c r="P36" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q36" s="21">
+        <v>0</v>
+      </c>
+      <c r="R36" s="20">
+        <v>0</v>
+      </c>
+      <c r="S36" s="3">
+        <v>0</v>
+      </c>
+      <c r="T36" s="21">
+        <v>1</v>
+      </c>
+      <c r="U36" s="7">
+        <v>0</v>
+      </c>
+      <c r="V36" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="W36" s="7">
+        <v>0</v>
+      </c>
+      <c r="X36" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE36" s="8" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="37" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A37" s="2"/>

</xml_diff>

<commit_message>
debug : [InvKinematics] : probrem = can't stack ik_data_st_ -> I generated and registered InvKinematics many times.
</commit_message>
<xml_diff>
--- a/gameCSV/Actor_RobotObj_01.xlsx
+++ b/gameCSV/Actor_RobotObj_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltz\Documents\CppProjects\GitManagements\QuantumCoreRobotReMake\gameCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{1D790327-7776-4AFF-A833-4A26CA8E86C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E09CA71-3876-4362-BD19-E1E542D21693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
+    <workbookView xWindow="2055" yWindow="6120" windowWidth="13875" windowHeight="10560" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
   </bookViews>
   <sheets>
     <sheet name="Actor_RobotObj_01" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
   <si>
     <t>id</t>
     <phoneticPr fontId="1"/>
@@ -239,10 +239,6 @@
     <phoneticPr fontId="1"/>
   </si>
   <si>
-    <t>Right Wrist Obj</t>
-    <phoneticPr fontId="1"/>
-  </si>
-  <si>
     <t>Right Wrist Tar</t>
     <phoneticPr fontId="1"/>
   </si>
@@ -292,6 +288,34 @@
   </si>
   <si>
     <t>non</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RAEE03</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>BD01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RA03</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Right Wrist Pos Obj</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Right Wrist Rot Obj</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>RATA03</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Right Wrist Pos Tar</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -682,7 +706,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -816,6 +840,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1135,8 +1162,8 @@
   <dimension ref="A1:AE104"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G34" sqref="G34"/>
+      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1432,7 +1459,7 @@
         <v>1</v>
       </c>
       <c r="AE4" s="21" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.4">
@@ -1527,7 +1554,7 @@
         <v>1</v>
       </c>
       <c r="AE5" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.4">
@@ -1622,7 +1649,7 @@
         <v>1</v>
       </c>
       <c r="AE6" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.4">
@@ -1903,7 +1930,7 @@
         <v>1</v>
       </c>
       <c r="AE9" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.4">
@@ -2184,7 +2211,7 @@
         <v>1</v>
       </c>
       <c r="AE12" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.4">
@@ -2372,7 +2399,7 @@
         <v>1</v>
       </c>
       <c r="AE14" s="8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.4">
@@ -2653,7 +2680,7 @@
         <v>1</v>
       </c>
       <c r="AE17" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.4">
@@ -3363,7 +3390,7 @@
         <v>1</v>
       </c>
       <c r="AE33" s="8" t="s">
-        <v>53</v>
+        <v>70</v>
       </c>
     </row>
     <row r="34" spans="1:31" x14ac:dyDescent="0.4">
@@ -3386,7 +3413,7 @@
         <v>8</v>
       </c>
       <c r="G34" s="8">
-        <v>3</v>
+        <v>2.8</v>
       </c>
       <c r="H34" s="20">
         <v>0</v>
@@ -3458,7 +3485,7 @@
         <v>1</v>
       </c>
       <c r="AE34" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="35" spans="1:31" x14ac:dyDescent="0.4">
@@ -3466,10 +3493,10 @@
         <v>1301</v>
       </c>
       <c r="B35" s="42" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C35" s="7">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="D35" s="6" t="s">
         <v>28</v>
@@ -3526,7 +3553,7 @@
         <v>0</v>
       </c>
       <c r="V35" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="W35" s="7">
         <v>0</v>
@@ -3553,7 +3580,7 @@
         <v>1</v>
       </c>
       <c r="AE35" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="36" spans="1:31" x14ac:dyDescent="0.4">
@@ -3561,7 +3588,7 @@
         <v>2301</v>
       </c>
       <c r="B36" s="43" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C36" s="7">
         <v>200</v>
@@ -3570,10 +3597,10 @@
         <v>24</v>
       </c>
       <c r="E36" s="7">
-        <v>3</v>
+        <v>2.7</v>
       </c>
       <c r="F36" s="2">
-        <v>8</v>
+        <v>8.5</v>
       </c>
       <c r="G36" s="8">
         <v>0</v>
@@ -3621,101 +3648,225 @@
         <v>0</v>
       </c>
       <c r="V36" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="W36" s="7">
+        <v>0</v>
+      </c>
+      <c r="X36" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y36" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB36" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD36" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE36" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="37" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A37" s="2">
+        <v>1302</v>
+      </c>
+      <c r="B37" s="42" t="s">
         <v>66</v>
       </c>
-      <c r="W36" s="7">
-        <v>0</v>
-      </c>
-      <c r="X36" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y36" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z36" s="7">
-        <v>0</v>
-      </c>
-      <c r="AA36" s="2">
-        <v>1</v>
-      </c>
-      <c r="AB36" s="2">
-        <v>0</v>
-      </c>
-      <c r="AC36" s="8">
-        <v>0</v>
-      </c>
-      <c r="AD36" s="8">
-        <v>1</v>
-      </c>
-      <c r="AE36" s="8" t="s">
+      <c r="C37" s="7">
+        <v>302</v>
+      </c>
+      <c r="D37" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="E37" s="7">
+        <v>2</v>
+      </c>
+      <c r="F37" s="2">
+        <v>6</v>
+      </c>
+      <c r="G37" s="8">
+        <v>0</v>
+      </c>
+      <c r="H37" s="20">
+        <v>0</v>
+      </c>
+      <c r="I37" s="3">
+        <v>1</v>
+      </c>
+      <c r="J37" s="3">
+        <v>0</v>
+      </c>
+      <c r="K37" s="21">
+        <v>0</v>
+      </c>
+      <c r="L37" s="20">
+        <v>1</v>
+      </c>
+      <c r="M37" s="3">
+        <v>0</v>
+      </c>
+      <c r="N37" s="21">
+        <v>0</v>
+      </c>
+      <c r="O37" s="20">
+        <v>0</v>
+      </c>
+      <c r="P37" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q37" s="21">
+        <v>0</v>
+      </c>
+      <c r="R37" s="20">
+        <v>0</v>
+      </c>
+      <c r="S37" s="3">
+        <v>0</v>
+      </c>
+      <c r="T37" s="21">
+        <v>1</v>
+      </c>
+      <c r="U37" s="7">
+        <v>0</v>
+      </c>
+      <c r="V37" s="8" t="s">
         <v>65</v>
       </c>
-    </row>
-    <row r="37" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A37" s="2"/>
-      <c r="B37" s="6"/>
-      <c r="C37" s="7"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="7"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="8"/>
-      <c r="H37" s="7"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="2"/>
-      <c r="K37" s="8"/>
-      <c r="L37" s="7"/>
-      <c r="M37" s="2"/>
-      <c r="N37" s="8"/>
-      <c r="O37" s="7"/>
-      <c r="P37" s="2"/>
-      <c r="Q37" s="8"/>
-      <c r="R37" s="7"/>
-      <c r="S37" s="2"/>
-      <c r="T37" s="8"/>
-      <c r="U37" s="7"/>
-      <c r="V37" s="8"/>
-      <c r="W37" s="7"/>
-      <c r="X37" s="2"/>
-      <c r="Y37" s="8"/>
-      <c r="Z37" s="7"/>
-      <c r="AA37" s="2"/>
-      <c r="AB37" s="2"/>
-      <c r="AC37" s="8"/>
-      <c r="AD37" s="8"/>
-      <c r="AE37" s="8"/>
+      <c r="W37" s="7">
+        <v>0</v>
+      </c>
+      <c r="X37" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y37" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB37" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD37" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE37" s="8" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="38" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A38" s="2"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="7"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="7"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="8"/>
-      <c r="H38" s="7"/>
-      <c r="I38" s="2"/>
-      <c r="J38" s="2"/>
-      <c r="K38" s="8"/>
-      <c r="L38" s="7"/>
-      <c r="M38" s="2"/>
-      <c r="N38" s="8"/>
-      <c r="O38" s="7"/>
-      <c r="P38" s="2"/>
-      <c r="Q38" s="8"/>
-      <c r="R38" s="7"/>
-      <c r="S38" s="2"/>
-      <c r="T38" s="8"/>
-      <c r="U38" s="7"/>
-      <c r="V38" s="8"/>
-      <c r="W38" s="7"/>
-      <c r="X38" s="2"/>
-      <c r="Y38" s="8"/>
-      <c r="Z38" s="7"/>
-      <c r="AA38" s="2"/>
-      <c r="AB38" s="2"/>
-      <c r="AC38" s="8"/>
-      <c r="AD38" s="8"/>
-      <c r="AE38" s="8"/>
+      <c r="A38" s="2">
+        <v>2302</v>
+      </c>
+      <c r="B38" s="45" t="s">
+        <v>71</v>
+      </c>
+      <c r="C38" s="7">
+        <v>200</v>
+      </c>
+      <c r="D38" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E38" s="7">
+        <v>2.2000000000000002</v>
+      </c>
+      <c r="F38" s="2">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G38" s="8">
+        <v>2</v>
+      </c>
+      <c r="H38" s="20">
+        <v>0</v>
+      </c>
+      <c r="I38" s="3">
+        <v>1</v>
+      </c>
+      <c r="J38" s="3">
+        <v>0</v>
+      </c>
+      <c r="K38" s="21">
+        <v>0</v>
+      </c>
+      <c r="L38" s="20">
+        <v>1</v>
+      </c>
+      <c r="M38" s="3">
+        <v>0</v>
+      </c>
+      <c r="N38" s="21">
+        <v>0</v>
+      </c>
+      <c r="O38" s="20">
+        <v>0</v>
+      </c>
+      <c r="P38" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q38" s="21">
+        <v>0</v>
+      </c>
+      <c r="R38" s="20">
+        <v>0</v>
+      </c>
+      <c r="S38" s="3">
+        <v>0</v>
+      </c>
+      <c r="T38" s="21">
+        <v>1</v>
+      </c>
+      <c r="U38" s="7">
+        <v>0</v>
+      </c>
+      <c r="V38" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="W38" s="7">
+        <v>0</v>
+      </c>
+      <c r="X38" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y38" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z38" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA38" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB38" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC38" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD38" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE38" s="8" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="39" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A39" s="2"/>

</xml_diff>

<commit_message>
add : [csv] : left arm ik setting.
</commit_message>
<xml_diff>
--- a/gameCSV/Actor_RobotObj_01.xlsx
+++ b/gameCSV/Actor_RobotObj_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltz\Documents\CppProjects\GitManagements\QuantumCoreRobotReMake\gameCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9E09CA71-3876-4362-BD19-E1E542D21693}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBF32037-57CA-4BE1-AB7D-BB91DA96E5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2055" yWindow="6120" windowWidth="13875" windowHeight="10560" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
+    <workbookView xWindow="-17340" yWindow="3090" windowWidth="17325" windowHeight="10560" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
   </bookViews>
   <sheets>
     <sheet name="Actor_RobotObj_01" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="86">
   <si>
     <t>id</t>
     <phoneticPr fontId="1"/>
@@ -316,6 +316,52 @@
   </si>
   <si>
     <t>Right Wrist Pos Tar</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>Left Wrist Rot Obj</t>
+  </si>
+  <si>
+    <t>Left Wrist Tar</t>
+  </si>
+  <si>
+    <t>Left elbow Obj</t>
+  </si>
+  <si>
+    <t>Left elbow Tar</t>
+  </si>
+  <si>
+    <t>Left Wrist Pos Obj</t>
+  </si>
+  <si>
+    <t>Left Wrist Pos Tar</t>
+  </si>
+  <si>
+    <t>LAEE01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LATA01</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LAEE02</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LATA02</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LAEE03</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LATA03</t>
+    <phoneticPr fontId="1"/>
+  </si>
+  <si>
+    <t>LA03</t>
     <phoneticPr fontId="1"/>
   </si>
 </sst>
@@ -1161,9 +1207,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70A82EBB-6C3C-46D3-B3DF-77C251B3AEE0}">
   <dimension ref="A1:AE104"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G36" sqref="G36"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1846,10 +1892,10 @@
         <v>30</v>
       </c>
       <c r="C9" s="7">
-        <v>100</v>
+        <v>200</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="E9" s="7">
         <v>-2</v>
@@ -4001,202 +4047,574 @@
       <c r="AE42" s="8"/>
     </row>
     <row r="43" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A43" s="2"/>
-      <c r="B43" s="6"/>
-      <c r="C43" s="7"/>
-      <c r="D43" s="6"/>
-      <c r="E43" s="7"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="8"/>
-      <c r="H43" s="7"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="8"/>
-      <c r="L43" s="7"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="8"/>
-      <c r="O43" s="7"/>
-      <c r="P43" s="2"/>
-      <c r="Q43" s="8"/>
-      <c r="R43" s="7"/>
-      <c r="S43" s="2"/>
-      <c r="T43" s="8"/>
-      <c r="U43" s="7"/>
-      <c r="V43" s="8"/>
-      <c r="W43" s="7"/>
-      <c r="X43" s="2"/>
-      <c r="Y43" s="8"/>
-      <c r="Z43" s="7"/>
-      <c r="AA43" s="2"/>
-      <c r="AB43" s="2"/>
-      <c r="AC43" s="8"/>
-      <c r="AD43" s="8"/>
-      <c r="AE43" s="8"/>
+      <c r="A43" s="2">
+        <v>1400</v>
+      </c>
+      <c r="B43" s="42" t="s">
+        <v>79</v>
+      </c>
+      <c r="C43" s="7">
+        <v>402</v>
+      </c>
+      <c r="D43" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="E43" s="7">
+        <v>-2</v>
+      </c>
+      <c r="F43" s="2">
+        <v>5.5</v>
+      </c>
+      <c r="G43" s="8">
+        <v>0</v>
+      </c>
+      <c r="H43" s="20">
+        <v>0</v>
+      </c>
+      <c r="I43" s="3">
+        <v>1</v>
+      </c>
+      <c r="J43" s="3">
+        <v>0</v>
+      </c>
+      <c r="K43" s="21">
+        <v>0</v>
+      </c>
+      <c r="L43" s="20">
+        <v>-1</v>
+      </c>
+      <c r="M43" s="3">
+        <v>0</v>
+      </c>
+      <c r="N43" s="21">
+        <v>0</v>
+      </c>
+      <c r="O43" s="20">
+        <v>0</v>
+      </c>
+      <c r="P43" s="3">
+        <v>-1</v>
+      </c>
+      <c r="Q43" s="21">
+        <v>0</v>
+      </c>
+      <c r="R43" s="20">
+        <v>0</v>
+      </c>
+      <c r="S43" s="3">
+        <v>0</v>
+      </c>
+      <c r="T43" s="21">
+        <v>-1</v>
+      </c>
+      <c r="U43" s="7">
+        <v>0</v>
+      </c>
+      <c r="V43" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="W43" s="20">
+        <v>0</v>
+      </c>
+      <c r="X43" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y43" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA43" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB43" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC43" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD43" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE43" s="8" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="44" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A44" s="2"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="7"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="7"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="8"/>
-      <c r="H44" s="7"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="8"/>
-      <c r="L44" s="7"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="8"/>
-      <c r="O44" s="7"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="8"/>
-      <c r="R44" s="7"/>
-      <c r="S44" s="2"/>
-      <c r="T44" s="8"/>
-      <c r="U44" s="7"/>
-      <c r="V44" s="8"/>
-      <c r="W44" s="7"/>
-      <c r="X44" s="2"/>
-      <c r="Y44" s="8"/>
-      <c r="Z44" s="7"/>
-      <c r="AA44" s="2"/>
-      <c r="AB44" s="2"/>
-      <c r="AC44" s="8"/>
-      <c r="AD44" s="8"/>
-      <c r="AE44" s="8"/>
+      <c r="A44" s="2">
+        <v>2400</v>
+      </c>
+      <c r="B44" s="43" t="s">
+        <v>80</v>
+      </c>
+      <c r="C44" s="7">
+        <v>0</v>
+      </c>
+      <c r="D44" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E44" s="7">
+        <v>-3</v>
+      </c>
+      <c r="F44" s="2">
+        <v>8</v>
+      </c>
+      <c r="G44" s="8">
+        <v>2.8</v>
+      </c>
+      <c r="H44" s="20">
+        <v>0</v>
+      </c>
+      <c r="I44" s="3">
+        <v>1</v>
+      </c>
+      <c r="J44" s="3">
+        <v>0</v>
+      </c>
+      <c r="K44" s="21">
+        <v>0</v>
+      </c>
+      <c r="L44" s="20">
+        <v>-1</v>
+      </c>
+      <c r="M44" s="3">
+        <v>0</v>
+      </c>
+      <c r="N44" s="21">
+        <v>0</v>
+      </c>
+      <c r="O44" s="20">
+        <v>0</v>
+      </c>
+      <c r="P44" s="3">
+        <v>-1</v>
+      </c>
+      <c r="Q44" s="21">
+        <v>0</v>
+      </c>
+      <c r="R44" s="20">
+        <v>0</v>
+      </c>
+      <c r="S44" s="3">
+        <v>0</v>
+      </c>
+      <c r="T44" s="21">
+        <v>-1</v>
+      </c>
+      <c r="U44" s="7">
+        <v>0</v>
+      </c>
+      <c r="V44" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="W44" s="20">
+        <v>0</v>
+      </c>
+      <c r="X44" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y44" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA44" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB44" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD44" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE44" s="8" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="45" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A45" s="2"/>
-      <c r="B45" s="6"/>
-      <c r="C45" s="7"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="7"/>
-      <c r="F45" s="2"/>
-      <c r="G45" s="8"/>
-      <c r="H45" s="7"/>
-      <c r="I45" s="2"/>
-      <c r="J45" s="2"/>
-      <c r="K45" s="8"/>
-      <c r="L45" s="7"/>
-      <c r="M45" s="2"/>
-      <c r="N45" s="8"/>
-      <c r="O45" s="7"/>
-      <c r="P45" s="2"/>
-      <c r="Q45" s="8"/>
-      <c r="R45" s="7"/>
-      <c r="S45" s="2"/>
-      <c r="T45" s="8"/>
-      <c r="U45" s="7"/>
-      <c r="V45" s="8"/>
-      <c r="W45" s="7"/>
-      <c r="X45" s="2"/>
-      <c r="Y45" s="8"/>
-      <c r="Z45" s="7"/>
-      <c r="AA45" s="2"/>
-      <c r="AB45" s="2"/>
-      <c r="AC45" s="8"/>
-      <c r="AD45" s="8"/>
-      <c r="AE45" s="8"/>
+      <c r="A45" s="2">
+        <v>1401</v>
+      </c>
+      <c r="B45" s="42" t="s">
+        <v>81</v>
+      </c>
+      <c r="C45" s="7">
+        <v>401</v>
+      </c>
+      <c r="D45" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="E45" s="7">
+        <v>-2</v>
+      </c>
+      <c r="F45" s="2">
+        <v>8</v>
+      </c>
+      <c r="G45" s="8">
+        <v>0</v>
+      </c>
+      <c r="H45" s="20">
+        <v>0</v>
+      </c>
+      <c r="I45" s="3">
+        <v>1</v>
+      </c>
+      <c r="J45" s="3">
+        <v>0</v>
+      </c>
+      <c r="K45" s="21">
+        <v>0</v>
+      </c>
+      <c r="L45" s="20">
+        <v>-1</v>
+      </c>
+      <c r="M45" s="3">
+        <v>0</v>
+      </c>
+      <c r="N45" s="21">
+        <v>0</v>
+      </c>
+      <c r="O45" s="20">
+        <v>0</v>
+      </c>
+      <c r="P45" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q45" s="21">
+        <v>0</v>
+      </c>
+      <c r="R45" s="20">
+        <v>0</v>
+      </c>
+      <c r="S45" s="3">
+        <v>0</v>
+      </c>
+      <c r="T45" s="21">
+        <v>1</v>
+      </c>
+      <c r="U45" s="7">
+        <v>0</v>
+      </c>
+      <c r="V45" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="W45" s="7">
+        <v>0</v>
+      </c>
+      <c r="X45" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y45" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA45" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB45" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD45" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE45" s="8" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="46" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A46" s="2"/>
-      <c r="B46" s="6"/>
-      <c r="C46" s="7"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="7"/>
-      <c r="F46" s="2"/>
-      <c r="G46" s="8"/>
-      <c r="H46" s="7"/>
-      <c r="I46" s="2"/>
-      <c r="J46" s="2"/>
-      <c r="K46" s="8"/>
-      <c r="L46" s="7"/>
-      <c r="M46" s="2"/>
-      <c r="N46" s="8"/>
-      <c r="O46" s="7"/>
-      <c r="P46" s="2"/>
-      <c r="Q46" s="8"/>
-      <c r="R46" s="7"/>
-      <c r="S46" s="2"/>
-      <c r="T46" s="8"/>
-      <c r="U46" s="7"/>
-      <c r="V46" s="8"/>
-      <c r="W46" s="7"/>
-      <c r="X46" s="2"/>
-      <c r="Y46" s="8"/>
-      <c r="Z46" s="7"/>
-      <c r="AA46" s="2"/>
-      <c r="AB46" s="2"/>
-      <c r="AC46" s="8"/>
-      <c r="AD46" s="8"/>
-      <c r="AE46" s="8"/>
+      <c r="A46" s="2">
+        <v>2401</v>
+      </c>
+      <c r="B46" s="43" t="s">
+        <v>82</v>
+      </c>
+      <c r="C46" s="7">
+        <v>200</v>
+      </c>
+      <c r="D46" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E46" s="7">
+        <v>-2.7</v>
+      </c>
+      <c r="F46" s="2">
+        <v>8.5</v>
+      </c>
+      <c r="G46" s="8">
+        <v>0</v>
+      </c>
+      <c r="H46" s="20">
+        <v>0</v>
+      </c>
+      <c r="I46" s="3">
+        <v>1</v>
+      </c>
+      <c r="J46" s="3">
+        <v>0</v>
+      </c>
+      <c r="K46" s="21">
+        <v>0</v>
+      </c>
+      <c r="L46" s="20">
+        <v>-1</v>
+      </c>
+      <c r="M46" s="3">
+        <v>0</v>
+      </c>
+      <c r="N46" s="21">
+        <v>0</v>
+      </c>
+      <c r="O46" s="20">
+        <v>0</v>
+      </c>
+      <c r="P46" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q46" s="21">
+        <v>0</v>
+      </c>
+      <c r="R46" s="20">
+        <v>0</v>
+      </c>
+      <c r="S46" s="3">
+        <v>0</v>
+      </c>
+      <c r="T46" s="21">
+        <v>1</v>
+      </c>
+      <c r="U46" s="7">
+        <v>0</v>
+      </c>
+      <c r="V46" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="W46" s="7">
+        <v>0</v>
+      </c>
+      <c r="X46" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y46" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA46" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB46" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC46" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD46" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE46" s="8" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="47" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A47" s="2"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="7"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="7"/>
-      <c r="F47" s="2"/>
-      <c r="G47" s="8"/>
-      <c r="H47" s="7"/>
-      <c r="I47" s="2"/>
-      <c r="J47" s="2"/>
-      <c r="K47" s="8"/>
-      <c r="L47" s="7"/>
-      <c r="M47" s="2"/>
-      <c r="N47" s="8"/>
-      <c r="O47" s="7"/>
-      <c r="P47" s="2"/>
-      <c r="Q47" s="8"/>
-      <c r="R47" s="7"/>
-      <c r="S47" s="2"/>
-      <c r="T47" s="8"/>
-      <c r="U47" s="7"/>
-      <c r="V47" s="8"/>
-      <c r="W47" s="7"/>
-      <c r="X47" s="2"/>
-      <c r="Y47" s="8"/>
-      <c r="Z47" s="7"/>
-      <c r="AA47" s="2"/>
-      <c r="AB47" s="2"/>
-      <c r="AC47" s="8"/>
-      <c r="AD47" s="8"/>
-      <c r="AE47" s="8"/>
+      <c r="A47" s="2">
+        <v>1402</v>
+      </c>
+      <c r="B47" s="42" t="s">
+        <v>83</v>
+      </c>
+      <c r="C47" s="7">
+        <v>402</v>
+      </c>
+      <c r="D47" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="E47" s="7">
+        <v>-2</v>
+      </c>
+      <c r="F47" s="2">
+        <v>6</v>
+      </c>
+      <c r="G47" s="8">
+        <v>0</v>
+      </c>
+      <c r="H47" s="20">
+        <v>0</v>
+      </c>
+      <c r="I47" s="3">
+        <v>1</v>
+      </c>
+      <c r="J47" s="3">
+        <v>0</v>
+      </c>
+      <c r="K47" s="21">
+        <v>0</v>
+      </c>
+      <c r="L47" s="20">
+        <v>-1</v>
+      </c>
+      <c r="M47" s="3">
+        <v>0</v>
+      </c>
+      <c r="N47" s="21">
+        <v>0</v>
+      </c>
+      <c r="O47" s="20">
+        <v>0</v>
+      </c>
+      <c r="P47" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q47" s="21">
+        <v>0</v>
+      </c>
+      <c r="R47" s="20">
+        <v>0</v>
+      </c>
+      <c r="S47" s="3">
+        <v>0</v>
+      </c>
+      <c r="T47" s="21">
+        <v>1</v>
+      </c>
+      <c r="U47" s="7">
+        <v>0</v>
+      </c>
+      <c r="V47" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="W47" s="7">
+        <v>0</v>
+      </c>
+      <c r="X47" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y47" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z47" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA47" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB47" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC47" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD47" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE47" s="8" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A48" s="2"/>
-      <c r="B48" s="6"/>
-      <c r="C48" s="7"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="7"/>
-      <c r="F48" s="2"/>
-      <c r="G48" s="8"/>
-      <c r="H48" s="7"/>
-      <c r="I48" s="2"/>
-      <c r="J48" s="2"/>
-      <c r="K48" s="8"/>
-      <c r="L48" s="7"/>
-      <c r="M48" s="2"/>
-      <c r="N48" s="8"/>
-      <c r="O48" s="7"/>
-      <c r="P48" s="2"/>
-      <c r="Q48" s="8"/>
-      <c r="R48" s="7"/>
-      <c r="S48" s="2"/>
-      <c r="T48" s="8"/>
-      <c r="U48" s="7"/>
-      <c r="V48" s="8"/>
-      <c r="W48" s="7"/>
-      <c r="X48" s="2"/>
-      <c r="Y48" s="8"/>
-      <c r="Z48" s="7"/>
-      <c r="AA48" s="2"/>
-      <c r="AB48" s="2"/>
-      <c r="AC48" s="8"/>
-      <c r="AD48" s="8"/>
-      <c r="AE48" s="8"/>
+      <c r="A48" s="2">
+        <v>2402</v>
+      </c>
+      <c r="B48" s="45" t="s">
+        <v>84</v>
+      </c>
+      <c r="C48" s="7">
+        <v>200</v>
+      </c>
+      <c r="D48" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E48" s="7">
+        <v>-2.2000000000000002</v>
+      </c>
+      <c r="F48" s="2">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="G48" s="8">
+        <v>2</v>
+      </c>
+      <c r="H48" s="20">
+        <v>0</v>
+      </c>
+      <c r="I48" s="3">
+        <v>1</v>
+      </c>
+      <c r="J48" s="3">
+        <v>0</v>
+      </c>
+      <c r="K48" s="21">
+        <v>0</v>
+      </c>
+      <c r="L48" s="20">
+        <v>-1</v>
+      </c>
+      <c r="M48" s="3">
+        <v>0</v>
+      </c>
+      <c r="N48" s="21">
+        <v>0</v>
+      </c>
+      <c r="O48" s="20">
+        <v>0</v>
+      </c>
+      <c r="P48" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q48" s="21">
+        <v>0</v>
+      </c>
+      <c r="R48" s="20">
+        <v>0</v>
+      </c>
+      <c r="S48" s="3">
+        <v>0</v>
+      </c>
+      <c r="T48" s="21">
+        <v>1</v>
+      </c>
+      <c r="U48" s="7">
+        <v>0</v>
+      </c>
+      <c r="V48" s="8" t="s">
+        <v>65</v>
+      </c>
+      <c r="W48" s="7">
+        <v>0</v>
+      </c>
+      <c r="X48" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y48" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z48" s="7">
+        <v>0</v>
+      </c>
+      <c r="AA48" s="2">
+        <v>1</v>
+      </c>
+      <c r="AB48" s="2">
+        <v>0</v>
+      </c>
+      <c r="AC48" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD48" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE48" s="8" t="s">
+        <v>78</v>
+      </c>
     </row>
     <row r="49" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A49" s="2"/>

</xml_diff>

<commit_message>
add : [csv] : head ik setting. (look target)
</commit_message>
<xml_diff>
--- a/gameCSV/Actor_RobotObj_01.xlsx
+++ b/gameCSV/Actor_RobotObj_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltz\Documents\CppProjects\GitManagements\QuantumCoreRobotReMake\gameCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EBF32037-57CA-4BE1-AB7D-BB91DA96E5C2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0DAD61C-6752-4D0D-90B5-16B4E36D5E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17340" yWindow="3090" windowWidth="17325" windowHeight="10560" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
+    <workbookView xWindow="-17040" yWindow="2745" windowWidth="17325" windowHeight="10560" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
   </bookViews>
   <sheets>
     <sheet name="Actor_RobotObj_01" sheetId="1" r:id="rId1"/>
@@ -1209,7 +1209,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D9" sqref="D9"/>
+      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1509,174 +1509,112 @@
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A5" s="2">
-        <v>200</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="C5" s="7">
-        <v>100</v>
-      </c>
-      <c r="D5" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="7">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>8</v>
-      </c>
-      <c r="G5" s="8">
-        <v>0</v>
-      </c>
-      <c r="H5" s="20">
-        <v>0</v>
-      </c>
-      <c r="I5" s="3">
-        <v>1</v>
-      </c>
-      <c r="J5" s="3">
-        <v>0</v>
-      </c>
-      <c r="K5" s="21">
-        <v>0</v>
-      </c>
-      <c r="L5" s="20">
-        <v>1</v>
-      </c>
-      <c r="M5" s="3">
-        <v>0</v>
-      </c>
-      <c r="N5" s="21">
-        <v>0</v>
-      </c>
-      <c r="O5" s="20">
-        <v>0</v>
-      </c>
-      <c r="P5" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q5" s="21">
-        <v>0</v>
-      </c>
-      <c r="R5" s="20">
-        <v>0</v>
-      </c>
-      <c r="S5" s="3">
-        <v>0</v>
-      </c>
-      <c r="T5" s="21">
-        <v>1</v>
-      </c>
-      <c r="U5" s="7">
-        <v>200</v>
-      </c>
-      <c r="V5" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="W5" s="7">
-        <v>0</v>
-      </c>
-      <c r="X5" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y5" s="8">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="3">
-        <v>1</v>
-      </c>
-      <c r="AB5" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC5" s="21">
-        <v>0</v>
-      </c>
-      <c r="AD5" s="21">
-        <v>1</v>
-      </c>
-      <c r="AE5" s="8" t="s">
-        <v>57</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="44"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="20"/>
+      <c r="I5" s="3"/>
+      <c r="J5" s="3"/>
+      <c r="K5" s="21"/>
+      <c r="L5" s="20"/>
+      <c r="M5" s="3"/>
+      <c r="N5" s="21"/>
+      <c r="O5" s="20"/>
+      <c r="P5" s="3"/>
+      <c r="Q5" s="21"/>
+      <c r="R5" s="20"/>
+      <c r="S5" s="3"/>
+      <c r="T5" s="21"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="8"/>
+      <c r="W5" s="20"/>
+      <c r="X5" s="3"/>
+      <c r="Y5" s="21"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="3"/>
+      <c r="AB5" s="3"/>
+      <c r="AC5" s="21"/>
+      <c r="AD5" s="21"/>
+      <c r="AE5" s="8"/>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
-        <v>300</v>
+        <v>200</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="20">
+        <v>24</v>
+      </c>
+      <c r="C6" s="7">
+        <v>100</v>
+      </c>
+      <c r="D6" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E6" s="7">
+        <v>0</v>
+      </c>
+      <c r="F6" s="2">
+        <v>8</v>
+      </c>
+      <c r="G6" s="8">
+        <v>0</v>
+      </c>
+      <c r="H6" s="20">
+        <v>0</v>
+      </c>
+      <c r="I6" s="3">
+        <v>1</v>
+      </c>
+      <c r="J6" s="3">
+        <v>0</v>
+      </c>
+      <c r="K6" s="21">
+        <v>0</v>
+      </c>
+      <c r="L6" s="20">
+        <v>1</v>
+      </c>
+      <c r="M6" s="3">
+        <v>0</v>
+      </c>
+      <c r="N6" s="21">
+        <v>0</v>
+      </c>
+      <c r="O6" s="20">
+        <v>0</v>
+      </c>
+      <c r="P6" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q6" s="21">
+        <v>0</v>
+      </c>
+      <c r="R6" s="20">
+        <v>0</v>
+      </c>
+      <c r="S6" s="3">
+        <v>0</v>
+      </c>
+      <c r="T6" s="21">
+        <v>1</v>
+      </c>
+      <c r="U6" s="7">
         <v>200</v>
       </c>
-      <c r="D6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E6" s="20">
-        <v>2</v>
-      </c>
-      <c r="F6" s="3">
-        <v>10</v>
-      </c>
-      <c r="G6" s="21">
-        <v>0</v>
-      </c>
-      <c r="H6" s="20">
-        <v>0</v>
-      </c>
-      <c r="I6" s="3">
-        <v>1</v>
-      </c>
-      <c r="J6" s="3">
-        <v>0</v>
-      </c>
-      <c r="K6" s="21">
-        <v>0</v>
-      </c>
-      <c r="L6" s="20">
-        <v>1</v>
-      </c>
-      <c r="M6" s="3">
-        <v>0</v>
-      </c>
-      <c r="N6" s="21">
-        <v>0</v>
-      </c>
-      <c r="O6" s="20">
-        <v>0</v>
-      </c>
-      <c r="P6" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q6" s="21">
-        <v>0</v>
-      </c>
-      <c r="R6" s="20">
-        <v>0</v>
-      </c>
-      <c r="S6" s="3">
-        <v>0</v>
-      </c>
-      <c r="T6" s="21">
-        <v>1</v>
-      </c>
-      <c r="U6" s="7">
-        <v>300</v>
-      </c>
       <c r="V6" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="W6" s="20">
-        <v>0</v>
-      </c>
-      <c r="X6" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="21">
+        <v>25</v>
+      </c>
+      <c r="W6" s="7">
+        <v>0</v>
+      </c>
+      <c r="X6" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="8">
         <v>0</v>
       </c>
       <c r="Z6" s="20">
@@ -1695,29 +1633,29 @@
         <v>1</v>
       </c>
       <c r="AE6" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C7" s="7">
-        <v>300</v>
+        <v>26</v>
+      </c>
+      <c r="C7" s="20">
+        <v>200</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E7" s="7">
+        <v>24</v>
+      </c>
+      <c r="E7" s="20">
         <v>2</v>
       </c>
-      <c r="F7" s="2">
-        <v>8</v>
-      </c>
-      <c r="G7" s="8">
+      <c r="F7" s="3">
+        <v>10</v>
+      </c>
+      <c r="G7" s="21">
         <v>0</v>
       </c>
       <c r="H7" s="20">
@@ -1765,13 +1703,13 @@
       <c r="V7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="W7" s="7">
-        <v>0</v>
-      </c>
-      <c r="X7" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="8">
+      <c r="W7" s="20">
+        <v>0</v>
+      </c>
+      <c r="X7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="21">
         <v>0</v>
       </c>
       <c r="Z7" s="20">
@@ -1789,28 +1727,30 @@
       <c r="AD7" s="21">
         <v>1</v>
       </c>
-      <c r="AE7" s="8"/>
+      <c r="AE7" s="8" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A8" s="2">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="20">
-        <v>301</v>
+        <v>28</v>
+      </c>
+      <c r="C8" s="7">
+        <v>300</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E8" s="20">
+        <v>26</v>
+      </c>
+      <c r="E8" s="7">
         <v>2</v>
       </c>
-      <c r="F8" s="3">
-        <v>6</v>
-      </c>
-      <c r="G8" s="21">
+      <c r="F8" s="2">
+        <v>8</v>
+      </c>
+      <c r="G8" s="8">
         <v>0</v>
       </c>
       <c r="H8" s="20">
@@ -1853,18 +1793,18 @@
         <v>1</v>
       </c>
       <c r="U8" s="7">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="V8" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="W8" s="20">
-        <v>0</v>
-      </c>
-      <c r="X8" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="21">
+        <v>27</v>
+      </c>
+      <c r="W8" s="7">
+        <v>0</v>
+      </c>
+      <c r="X8" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="8">
         <v>0</v>
       </c>
       <c r="Z8" s="20">
@@ -1879,31 +1819,31 @@
       <c r="AC8" s="21">
         <v>0</v>
       </c>
-      <c r="AD8" s="8">
+      <c r="AD8" s="21">
         <v>1</v>
       </c>
       <c r="AE8" s="8"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
-        <v>400</v>
+        <v>302</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="C9" s="7">
-        <v>200</v>
+        <v>29</v>
+      </c>
+      <c r="C9" s="20">
+        <v>301</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E9" s="7">
-        <v>-2</v>
-      </c>
-      <c r="F9" s="2">
-        <v>10</v>
-      </c>
-      <c r="G9" s="8">
+        <v>28</v>
+      </c>
+      <c r="E9" s="20">
+        <v>2</v>
+      </c>
+      <c r="F9" s="3">
+        <v>6</v>
+      </c>
+      <c r="G9" s="21">
         <v>0</v>
       </c>
       <c r="H9" s="20">
@@ -1946,10 +1886,10 @@
         <v>1</v>
       </c>
       <c r="U9" s="7">
-        <v>400</v>
+        <v>301</v>
       </c>
       <c r="V9" s="8" t="s">
-        <v>31</v>
+        <v>50</v>
       </c>
       <c r="W9" s="20">
         <v>0</v>
@@ -1975,28 +1915,26 @@
       <c r="AD9" s="8">
         <v>1</v>
       </c>
-      <c r="AE9" s="8" t="s">
-        <v>59</v>
-      </c>
+      <c r="AE9" s="8"/>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A10" s="2">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" s="7">
-        <v>400</v>
+        <v>200</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E10" s="7">
         <v>-2</v>
       </c>
       <c r="F10" s="2">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="G10" s="8">
         <v>0</v>
@@ -2070,26 +2008,28 @@
       <c r="AD10" s="8">
         <v>1</v>
       </c>
-      <c r="AE10" s="8"/>
+      <c r="AE10" s="8" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A11" s="2">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C11" s="7">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E11" s="7">
         <v>-2</v>
       </c>
       <c r="F11" s="2">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="G11" s="8">
         <v>0</v>
@@ -2134,10 +2074,10 @@
         <v>1</v>
       </c>
       <c r="U11" s="7">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="V11" s="8" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="W11" s="20">
         <v>0</v>
@@ -2167,22 +2107,22 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A12" s="2">
-        <v>500</v>
+        <v>402</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C12" s="7">
-        <v>100</v>
+        <v>401</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="E12" s="7">
-        <v>0</v>
+        <v>-2</v>
       </c>
       <c r="F12" s="2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G12" s="8">
         <v>0</v>
@@ -2227,10 +2167,10 @@
         <v>1</v>
       </c>
       <c r="U12" s="7">
-        <v>500</v>
+        <v>401</v>
       </c>
       <c r="V12" s="8" t="s">
-        <v>36</v>
+        <v>51</v>
       </c>
       <c r="W12" s="20">
         <v>0</v>
@@ -2256,76 +2196,74 @@
       <c r="AD12" s="8">
         <v>1</v>
       </c>
-      <c r="AE12" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="AE12" s="8"/>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
-        <v>501</v>
+        <v>500</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C13" s="7">
+        <v>100</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="7">
+        <v>0</v>
+      </c>
+      <c r="F13" s="2">
+        <v>10</v>
+      </c>
+      <c r="G13" s="8">
+        <v>0</v>
+      </c>
+      <c r="H13" s="20">
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <v>1</v>
+      </c>
+      <c r="J13" s="3">
+        <v>0</v>
+      </c>
+      <c r="K13" s="21">
+        <v>0</v>
+      </c>
+      <c r="L13" s="20">
+        <v>1</v>
+      </c>
+      <c r="M13" s="3">
+        <v>0</v>
+      </c>
+      <c r="N13" s="21">
+        <v>0</v>
+      </c>
+      <c r="O13" s="20">
+        <v>0</v>
+      </c>
+      <c r="P13" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q13" s="21">
+        <v>0</v>
+      </c>
+      <c r="R13" s="20">
+        <v>0</v>
+      </c>
+      <c r="S13" s="3">
+        <v>0</v>
+      </c>
+      <c r="T13" s="21">
+        <v>1</v>
+      </c>
+      <c r="U13" s="7">
         <v>500</v>
       </c>
-      <c r="D13" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="E13" s="7">
-        <v>0</v>
-      </c>
-      <c r="F13" s="2">
-        <v>10.75</v>
-      </c>
-      <c r="G13" s="8">
-        <v>0</v>
-      </c>
-      <c r="H13" s="20">
-        <v>0</v>
-      </c>
-      <c r="I13" s="3">
-        <v>1</v>
-      </c>
-      <c r="J13" s="3">
-        <v>0</v>
-      </c>
-      <c r="K13" s="21">
-        <v>0</v>
-      </c>
-      <c r="L13" s="20">
-        <v>1</v>
-      </c>
-      <c r="M13" s="3">
-        <v>0</v>
-      </c>
-      <c r="N13" s="21">
-        <v>0</v>
-      </c>
-      <c r="O13" s="20">
-        <v>0</v>
-      </c>
-      <c r="P13" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q13" s="21">
-        <v>0</v>
-      </c>
-      <c r="R13" s="20">
-        <v>0</v>
-      </c>
-      <c r="S13" s="3">
-        <v>0</v>
-      </c>
-      <c r="T13" s="21">
-        <v>1</v>
-      </c>
-      <c r="U13" s="7">
-        <v>501</v>
-      </c>
       <c r="V13" s="8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="W13" s="20">
         <v>0</v>
@@ -2351,26 +2289,28 @@
       <c r="AD13" s="8">
         <v>1</v>
       </c>
-      <c r="AE13" s="8"/>
+      <c r="AE13" s="8" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
-        <v>600</v>
+        <v>501</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C14" s="7">
-        <v>200</v>
+        <v>500</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>24</v>
+        <v>34</v>
       </c>
       <c r="E14" s="7">
-        <v>1.5</v>
+        <v>0</v>
       </c>
       <c r="F14" s="2">
-        <v>6</v>
+        <v>10.75</v>
       </c>
       <c r="G14" s="8">
         <v>0</v>
@@ -2415,10 +2355,10 @@
         <v>1</v>
       </c>
       <c r="U14" s="7">
-        <v>600</v>
+        <v>501</v>
       </c>
       <c r="V14" s="8" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="W14" s="20">
         <v>0</v>
@@ -2444,28 +2384,26 @@
       <c r="AD14" s="8">
         <v>1</v>
       </c>
-      <c r="AE14" s="8" t="s">
-        <v>61</v>
-      </c>
+      <c r="AE14" s="8"/>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A15" s="2">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="B15" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C15" s="7">
-        <v>600</v>
+        <v>200</v>
       </c>
       <c r="D15" s="6" t="s">
-        <v>38</v>
+        <v>24</v>
       </c>
       <c r="E15" s="7">
         <v>1.5</v>
       </c>
       <c r="F15" s="2">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="G15" s="8">
         <v>0</v>
@@ -2539,26 +2477,28 @@
       <c r="AD15" s="8">
         <v>1</v>
       </c>
-      <c r="AE15" s="8"/>
+      <c r="AE15" s="8" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A16" s="2">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C16" s="7">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E16" s="7">
         <v>1.5</v>
       </c>
       <c r="F16" s="2">
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="G16" s="8">
         <v>0</v>
@@ -2603,10 +2543,10 @@
         <v>1</v>
       </c>
       <c r="U16" s="7">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="V16" s="8" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="W16" s="20">
         <v>0</v>
@@ -2636,22 +2576,22 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A17" s="2">
-        <v>700</v>
+        <v>602</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C17" s="7">
-        <v>200</v>
+        <v>601</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>24</v>
+        <v>40</v>
       </c>
       <c r="E17" s="7">
-        <v>-1.5</v>
+        <v>1.5</v>
       </c>
       <c r="F17" s="2">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G17" s="8">
         <v>0</v>
@@ -2696,10 +2636,10 @@
         <v>1</v>
       </c>
       <c r="U17" s="7">
-        <v>700</v>
+        <v>601</v>
       </c>
       <c r="V17" s="8" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="W17" s="20">
         <v>0</v>
@@ -2725,28 +2665,26 @@
       <c r="AD17" s="8">
         <v>1</v>
       </c>
-      <c r="AE17" s="8" t="s">
-        <v>62</v>
-      </c>
+      <c r="AE17" s="8"/>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A18" s="2">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C18" s="7">
-        <v>700</v>
+        <v>200</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="E18" s="7">
         <v>-1.5</v>
       </c>
       <c r="F18" s="2">
-        <v>3.5</v>
+        <v>6</v>
       </c>
       <c r="G18" s="8">
         <v>0</v>
@@ -2820,26 +2758,28 @@
       <c r="AD18" s="8">
         <v>1</v>
       </c>
-      <c r="AE18" s="8"/>
+      <c r="AE18" s="8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A19" s="2">
-        <v>702</v>
+        <v>701</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19" s="7">
-        <v>701</v>
+        <v>700</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="E19" s="7">
         <v>-1.5</v>
       </c>
       <c r="F19" s="2">
-        <v>1</v>
+        <v>3.5</v>
       </c>
       <c r="G19" s="8">
         <v>0</v>
@@ -2884,68 +2824,128 @@
         <v>1</v>
       </c>
       <c r="U19" s="7">
+        <v>700</v>
+      </c>
+      <c r="V19" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="W19" s="20">
+        <v>0</v>
+      </c>
+      <c r="X19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y19" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB19" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD19" s="8">
+        <v>1</v>
+      </c>
+      <c r="AE19" s="8"/>
+    </row>
+    <row r="20" spans="1:31" x14ac:dyDescent="0.4">
+      <c r="A20" s="2">
+        <v>702</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C20" s="7">
         <v>701</v>
       </c>
-      <c r="V19" s="8" t="s">
+      <c r="D20" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="E20" s="7">
+        <v>-1.5</v>
+      </c>
+      <c r="F20" s="2">
+        <v>1</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+      <c r="H20" s="20">
+        <v>0</v>
+      </c>
+      <c r="I20" s="3">
+        <v>1</v>
+      </c>
+      <c r="J20" s="3">
+        <v>0</v>
+      </c>
+      <c r="K20" s="21">
+        <v>0</v>
+      </c>
+      <c r="L20" s="20">
+        <v>1</v>
+      </c>
+      <c r="M20" s="3">
+        <v>0</v>
+      </c>
+      <c r="N20" s="21">
+        <v>0</v>
+      </c>
+      <c r="O20" s="20">
+        <v>0</v>
+      </c>
+      <c r="P20" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q20" s="21">
+        <v>0</v>
+      </c>
+      <c r="R20" s="20">
+        <v>0</v>
+      </c>
+      <c r="S20" s="3">
+        <v>0</v>
+      </c>
+      <c r="T20" s="21">
+        <v>1</v>
+      </c>
+      <c r="U20" s="7">
+        <v>701</v>
+      </c>
+      <c r="V20" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="W19" s="20">
-        <v>0</v>
-      </c>
-      <c r="X19" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y19" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="3">
-        <v>1</v>
-      </c>
-      <c r="AB19" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC19" s="21">
-        <v>0</v>
-      </c>
-      <c r="AD19" s="8">
-        <v>1</v>
-      </c>
-      <c r="AE19" s="8"/>
-    </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A20" s="2"/>
-      <c r="B20" s="44"/>
-      <c r="C20" s="7"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="7"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="8"/>
-      <c r="H20" s="20"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="20"/>
-      <c r="M20" s="3"/>
-      <c r="N20" s="21"/>
-      <c r="O20" s="20"/>
-      <c r="P20" s="3"/>
-      <c r="Q20" s="21"/>
-      <c r="R20" s="20"/>
-      <c r="S20" s="3"/>
-      <c r="T20" s="21"/>
-      <c r="U20" s="7"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="20"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="21"/>
-      <c r="Z20" s="20"/>
-      <c r="AA20" s="3"/>
-      <c r="AB20" s="3"/>
-      <c r="AC20" s="21"/>
-      <c r="AD20" s="8"/>
+      <c r="W20" s="20">
+        <v>0</v>
+      </c>
+      <c r="X20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="21">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB20" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD20" s="8">
+        <v>1</v>
+      </c>
       <c r="AE20" s="8"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.4">

</xml_diff>

<commit_message>
add: [Weapon] : create bullet generate func.
</commit_message>
<xml_diff>
--- a/gameCSV/Actor_RobotObj_01.xlsx
+++ b/gameCSV/Actor_RobotObj_01.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltz\Documents\CppProjects\GitManagements\QuantumCoreRobotReMake\gameCSV\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B0DAD61C-6752-4D0D-90B5-16B4E36D5E31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{4991A691-4E1E-4A69-B84E-C67AFFA6B313}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-17040" yWindow="2745" windowWidth="17325" windowHeight="10560" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
+    <workbookView xWindow="13470" yWindow="5220" windowWidth="17325" windowHeight="10560" xr2:uid="{4A88D659-4C13-44B6-A2BE-41980A9F7671}"/>
   </bookViews>
   <sheets>
     <sheet name="Actor_RobotObj_01" sheetId="1" r:id="rId1"/>
@@ -1209,7 +1209,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D6" sqref="D6"/>
+      <selection pane="bottomLeft" activeCell="T13" sqref="T13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
@@ -1509,58 +1509,120 @@
       </c>
     </row>
     <row r="5" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A5" s="2"/>
-      <c r="B5" s="44"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="7"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="20"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="21"/>
-      <c r="L5" s="20"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="21"/>
-      <c r="O5" s="20"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="21"/>
-      <c r="R5" s="20"/>
-      <c r="S5" s="3"/>
-      <c r="T5" s="21"/>
-      <c r="U5" s="7"/>
-      <c r="V5" s="8"/>
-      <c r="W5" s="20"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="21"/>
-      <c r="Z5" s="20"/>
-      <c r="AA5" s="3"/>
-      <c r="AB5" s="3"/>
-      <c r="AC5" s="21"/>
-      <c r="AD5" s="21"/>
-      <c r="AE5" s="8"/>
+      <c r="A5" s="2">
+        <v>200</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="7">
+        <v>100</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" s="7">
+        <v>0</v>
+      </c>
+      <c r="F5" s="2">
+        <v>8</v>
+      </c>
+      <c r="G5" s="8">
+        <v>0</v>
+      </c>
+      <c r="H5" s="20">
+        <v>0</v>
+      </c>
+      <c r="I5" s="3">
+        <v>1</v>
+      </c>
+      <c r="J5" s="3">
+        <v>0</v>
+      </c>
+      <c r="K5" s="21">
+        <v>0</v>
+      </c>
+      <c r="L5" s="20">
+        <v>1</v>
+      </c>
+      <c r="M5" s="3">
+        <v>0</v>
+      </c>
+      <c r="N5" s="21">
+        <v>0</v>
+      </c>
+      <c r="O5" s="20">
+        <v>0</v>
+      </c>
+      <c r="P5" s="3">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="21">
+        <v>0</v>
+      </c>
+      <c r="R5" s="20">
+        <v>0</v>
+      </c>
+      <c r="S5" s="3">
+        <v>0</v>
+      </c>
+      <c r="T5" s="21">
+        <v>1</v>
+      </c>
+      <c r="U5" s="7">
+        <v>200</v>
+      </c>
+      <c r="V5" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="W5" s="7">
+        <v>0</v>
+      </c>
+      <c r="X5" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y5" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="20">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="3">
+        <v>1</v>
+      </c>
+      <c r="AB5" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="21">
+        <v>0</v>
+      </c>
+      <c r="AD5" s="21">
+        <v>1</v>
+      </c>
+      <c r="AE5" s="8" t="s">
+        <v>57</v>
+      </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A6" s="2">
+        <v>300</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="20">
         <v>200</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="D6" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="7">
-        <v>100</v>
-      </c>
-      <c r="D6" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="E6" s="7">
-        <v>0</v>
-      </c>
-      <c r="F6" s="2">
-        <v>8</v>
-      </c>
-      <c r="G6" s="8">
+      <c r="E6" s="20">
+        <v>2</v>
+      </c>
+      <c r="F6" s="3">
+        <v>10</v>
+      </c>
+      <c r="G6" s="21">
         <v>0</v>
       </c>
       <c r="H6" s="20">
@@ -1603,18 +1665,18 @@
         <v>1</v>
       </c>
       <c r="U6" s="7">
-        <v>200</v>
+        <v>300</v>
       </c>
       <c r="V6" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="W6" s="7">
-        <v>0</v>
-      </c>
-      <c r="X6" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y6" s="8">
+        <v>27</v>
+      </c>
+      <c r="W6" s="20">
+        <v>0</v>
+      </c>
+      <c r="X6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y6" s="21">
         <v>0</v>
       </c>
       <c r="Z6" s="20">
@@ -1633,29 +1695,29 @@
         <v>1</v>
       </c>
       <c r="AE6" s="8" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A7" s="2">
+        <v>301</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" s="7">
         <v>300</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="D7" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C7" s="20">
-        <v>200</v>
-      </c>
-      <c r="D7" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="E7" s="20">
+      <c r="E7" s="7">
         <v>2</v>
       </c>
-      <c r="F7" s="3">
-        <v>10</v>
-      </c>
-      <c r="G7" s="21">
+      <c r="F7" s="2">
+        <v>8</v>
+      </c>
+      <c r="G7" s="8">
         <v>0</v>
       </c>
       <c r="H7" s="20">
@@ -1703,13 +1765,13 @@
       <c r="V7" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="W7" s="20">
-        <v>0</v>
-      </c>
-      <c r="X7" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y7" s="21">
+      <c r="W7" s="7">
+        <v>0</v>
+      </c>
+      <c r="X7" s="2">
+        <v>0</v>
+      </c>
+      <c r="Y7" s="8">
         <v>0</v>
       </c>
       <c r="Z7" s="20">
@@ -1727,30 +1789,28 @@
       <c r="AD7" s="21">
         <v>1</v>
       </c>
-      <c r="AE7" s="8" t="s">
-        <v>58</v>
-      </c>
+      <c r="AE7" s="8"/>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A8" s="2">
+        <v>302</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C8" s="20">
         <v>301</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C8" s="7">
-        <v>300</v>
-      </c>
-      <c r="D8" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="E8" s="7">
+      <c r="E8" s="20">
         <v>2</v>
       </c>
-      <c r="F8" s="2">
-        <v>8</v>
-      </c>
-      <c r="G8" s="8">
+      <c r="F8" s="3">
+        <v>6</v>
+      </c>
+      <c r="G8" s="21">
         <v>0</v>
       </c>
       <c r="H8" s="20">
@@ -1793,18 +1853,18 @@
         <v>1</v>
       </c>
       <c r="U8" s="7">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="V8" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="W8" s="7">
-        <v>0</v>
-      </c>
-      <c r="X8" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="8">
+        <v>50</v>
+      </c>
+      <c r="W8" s="20">
+        <v>0</v>
+      </c>
+      <c r="X8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="21">
         <v>0</v>
       </c>
       <c r="Z8" s="20">
@@ -1819,31 +1879,31 @@
       <c r="AC8" s="21">
         <v>0</v>
       </c>
-      <c r="AD8" s="21">
+      <c r="AD8" s="8">
         <v>1</v>
       </c>
       <c r="AE8" s="8"/>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A9" s="2">
-        <v>302</v>
+        <v>400</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C9" s="20">
-        <v>301</v>
+        <v>30</v>
+      </c>
+      <c r="C9" s="7">
+        <v>200</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="E9" s="20">
-        <v>2</v>
-      </c>
-      <c r="F9" s="3">
-        <v>6</v>
-      </c>
-      <c r="G9" s="21">
+        <v>24</v>
+      </c>
+      <c r="E9" s="7">
+        <v>-2</v>
+      </c>
+      <c r="F9" s="2">
+        <v>10</v>
+      </c>
+      <c r="G9" s="8">
         <v>0</v>
       </c>
       <c r="H9" s="20">
@@ -1886,10 +1946,10 @@
         <v>1</v>
       </c>
       <c r="U9" s="7">
-        <v>301</v>
+        <v>400</v>
       </c>
       <c r="V9" s="8" t="s">
-        <v>50</v>
+        <v>31</v>
       </c>
       <c r="W9" s="20">
         <v>0</v>
@@ -1915,26 +1975,28 @@
       <c r="AD9" s="8">
         <v>1</v>
       </c>
-      <c r="AE9" s="8"/>
+      <c r="AE9" s="8" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A10" s="2">
+        <v>401</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C10" s="7">
         <v>400</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="D10" s="6" t="s">
         <v>30</v>
-      </c>
-      <c r="C10" s="7">
-        <v>200</v>
-      </c>
-      <c r="D10" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E10" s="7">
         <v>-2</v>
       </c>
       <c r="F10" s="2">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="G10" s="8">
         <v>0</v>
@@ -2008,28 +2070,26 @@
       <c r="AD10" s="8">
         <v>1</v>
       </c>
-      <c r="AE10" s="8" t="s">
-        <v>59</v>
-      </c>
+      <c r="AE10" s="8"/>
     </row>
     <row r="11" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A11" s="2">
+        <v>402</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="7">
         <v>401</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="D11" s="6" t="s">
         <v>32</v>
-      </c>
-      <c r="C11" s="7">
-        <v>400</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>30</v>
       </c>
       <c r="E11" s="7">
         <v>-2</v>
       </c>
       <c r="F11" s="2">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="G11" s="8">
         <v>0</v>
@@ -2074,10 +2134,10 @@
         <v>1</v>
       </c>
       <c r="U11" s="7">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="V11" s="8" t="s">
-        <v>31</v>
+        <v>51</v>
       </c>
       <c r="W11" s="20">
         <v>0</v>
@@ -2107,22 +2167,22 @@
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A12" s="2">
-        <v>402</v>
+        <v>500</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="C12" s="7">
-        <v>401</v>
+        <v>100</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="E12" s="7">
-        <v>-2</v>
+        <v>0</v>
       </c>
       <c r="F12" s="2">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G12" s="8">
         <v>0</v>
@@ -2167,10 +2227,10 @@
         <v>1</v>
       </c>
       <c r="U12" s="7">
-        <v>401</v>
+        <v>500</v>
       </c>
       <c r="V12" s="8" t="s">
-        <v>51</v>
+        <v>36</v>
       </c>
       <c r="W12" s="20">
         <v>0</v>
@@ -2196,26 +2256,28 @@
       <c r="AD12" s="8">
         <v>1</v>
       </c>
-      <c r="AE12" s="8"/>
+      <c r="AE12" s="8" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A13" s="2">
+        <v>501</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C13" s="7">
         <v>500</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="D13" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C13" s="7">
-        <v>100</v>
-      </c>
-      <c r="D13" s="6" t="s">
-        <v>21</v>
-      </c>
       <c r="E13" s="7">
         <v>0</v>
       </c>
       <c r="F13" s="2">
-        <v>10</v>
+        <v>10.75</v>
       </c>
       <c r="G13" s="8">
         <v>0</v>
@@ -2260,10 +2322,10 @@
         <v>1</v>
       </c>
       <c r="U13" s="7">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="V13" s="8" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="W13" s="20">
         <v>0</v>
@@ -2289,28 +2351,26 @@
       <c r="AD13" s="8">
         <v>1</v>
       </c>
-      <c r="AE13" s="8" t="s">
-        <v>60</v>
-      </c>
+      <c r="AE13" s="8"/>
     </row>
     <row r="14" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A14" s="2">
-        <v>501</v>
+        <v>600</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="C14" s="7">
-        <v>500</v>
+        <v>200</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>34</v>
+        <v>24</v>
       </c>
       <c r="E14" s="7">
-        <v>0</v>
+        <v>1.5</v>
       </c>
       <c r="F14" s="2">
-        <v>10.75</v>
+        <v>6</v>
       </c>
       <c r="G14" s="8">
         <v>0</v>
@@ -2355,10 +2415,10 @@
         <v>1</v>
       </c>
       <c r="U14" s="7">
-        <v>501</v>
+        <v>600</v>
       </c>
       <c r="V14" s="8" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="W14" s="20">
         <v>0</v>
@@ -2384,26 +2444,28 @@
       <c r="AD14" s="8">
         <v>1</v>
       </c>
-      <c r="AE14" s="8"/>
+      <c r="AE14" s="8" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A15" s="2">
+        <v>601</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C15" s="7">
         <v>600</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="D15" s="6" t="s">
         <v>38</v>
-      </c>
-      <c r="C15" s="7">
-        <v>200</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E15" s="7">
         <v>1.5</v>
       </c>
       <c r="F15" s="2">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="G15" s="8">
         <v>0</v>
@@ -2477,28 +2539,26 @@
       <c r="AD15" s="8">
         <v>1</v>
       </c>
-      <c r="AE15" s="8" t="s">
-        <v>61</v>
-      </c>
+      <c r="AE15" s="8"/>
     </row>
     <row r="16" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A16" s="2">
+        <v>602</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" s="7">
         <v>601</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="D16" s="6" t="s">
         <v>40</v>
-      </c>
-      <c r="C16" s="7">
-        <v>600</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>38</v>
       </c>
       <c r="E16" s="7">
         <v>1.5</v>
       </c>
       <c r="F16" s="2">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="G16" s="8">
         <v>0</v>
@@ -2543,10 +2603,10 @@
         <v>1</v>
       </c>
       <c r="U16" s="7">
-        <v>600</v>
+        <v>601</v>
       </c>
       <c r="V16" s="8" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="W16" s="20">
         <v>0</v>
@@ -2576,22 +2636,22 @@
     </row>
     <row r="17" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A17" s="2">
-        <v>602</v>
+        <v>700</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="C17" s="7">
-        <v>601</v>
+        <v>200</v>
       </c>
       <c r="D17" s="6" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E17" s="7">
-        <v>1.5</v>
+        <v>-1.5</v>
       </c>
       <c r="F17" s="2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G17" s="8">
         <v>0</v>
@@ -2636,10 +2696,10 @@
         <v>1</v>
       </c>
       <c r="U17" s="7">
-        <v>601</v>
+        <v>700</v>
       </c>
       <c r="V17" s="8" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="W17" s="20">
         <v>0</v>
@@ -2665,26 +2725,28 @@
       <c r="AD17" s="8">
         <v>1</v>
       </c>
-      <c r="AE17" s="8"/>
+      <c r="AE17" s="8" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="18" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A18" s="2">
+        <v>701</v>
+      </c>
+      <c r="B18" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C18" s="7">
         <v>700</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="D18" s="6" t="s">
         <v>43</v>
-      </c>
-      <c r="C18" s="7">
-        <v>200</v>
-      </c>
-      <c r="D18" s="6" t="s">
-        <v>24</v>
       </c>
       <c r="E18" s="7">
         <v>-1.5</v>
       </c>
       <c r="F18" s="2">
-        <v>6</v>
+        <v>3.5</v>
       </c>
       <c r="G18" s="8">
         <v>0</v>
@@ -2758,28 +2820,26 @@
       <c r="AD18" s="8">
         <v>1</v>
       </c>
-      <c r="AE18" s="8" t="s">
-        <v>62</v>
-      </c>
+      <c r="AE18" s="8"/>
     </row>
     <row r="19" spans="1:31" x14ac:dyDescent="0.4">
       <c r="A19" s="2">
+        <v>702</v>
+      </c>
+      <c r="B19" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" s="7">
         <v>701</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="D19" s="6" t="s">
         <v>45</v>
-      </c>
-      <c r="C19" s="7">
-        <v>700</v>
-      </c>
-      <c r="D19" s="6" t="s">
-        <v>43</v>
       </c>
       <c r="E19" s="7">
         <v>-1.5</v>
       </c>
       <c r="F19" s="2">
-        <v>3.5</v>
+        <v>1</v>
       </c>
       <c r="G19" s="8">
         <v>0</v>
@@ -2824,10 +2884,10 @@
         <v>1</v>
       </c>
       <c r="U19" s="7">
-        <v>700</v>
+        <v>701</v>
       </c>
       <c r="V19" s="8" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="W19" s="20">
         <v>0</v>
@@ -2856,96 +2916,36 @@
       <c r="AE19" s="8"/>
     </row>
     <row r="20" spans="1:31" x14ac:dyDescent="0.4">
-      <c r="A20" s="2">
-        <v>702</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C20" s="7">
-        <v>701</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="E20" s="7">
-        <v>-1.5</v>
-      </c>
-      <c r="F20" s="2">
-        <v>1</v>
-      </c>
-      <c r="G20" s="8">
-        <v>0</v>
-      </c>
-      <c r="H20" s="20">
-        <v>0</v>
-      </c>
-      <c r="I20" s="3">
-        <v>1</v>
-      </c>
-      <c r="J20" s="3">
-        <v>0</v>
-      </c>
-      <c r="K20" s="21">
-        <v>0</v>
-      </c>
-      <c r="L20" s="20">
-        <v>1</v>
-      </c>
-      <c r="M20" s="3">
-        <v>0</v>
-      </c>
-      <c r="N20" s="21">
-        <v>0</v>
-      </c>
-      <c r="O20" s="20">
-        <v>0</v>
-      </c>
-      <c r="P20" s="3">
-        <v>1</v>
-      </c>
-      <c r="Q20" s="21">
-        <v>0</v>
-      </c>
-      <c r="R20" s="20">
-        <v>0</v>
-      </c>
-      <c r="S20" s="3">
-        <v>0</v>
-      </c>
-      <c r="T20" s="21">
-        <v>1</v>
-      </c>
-      <c r="U20" s="7">
-        <v>701</v>
-      </c>
-      <c r="V20" s="8" t="s">
-        <v>47</v>
-      </c>
-      <c r="W20" s="20">
-        <v>0</v>
-      </c>
-      <c r="X20" s="3">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="21">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="20">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="3">
-        <v>1</v>
-      </c>
-      <c r="AB20" s="3">
-        <v>0</v>
-      </c>
-      <c r="AC20" s="21">
-        <v>0</v>
-      </c>
-      <c r="AD20" s="8">
-        <v>1</v>
-      </c>
+      <c r="A20" s="2"/>
+      <c r="B20" s="44"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="7"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="8"/>
+      <c r="H20" s="20"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="21"/>
+      <c r="L20" s="20"/>
+      <c r="M20" s="3"/>
+      <c r="N20" s="21"/>
+      <c r="O20" s="20"/>
+      <c r="P20" s="3"/>
+      <c r="Q20" s="21"/>
+      <c r="R20" s="20"/>
+      <c r="S20" s="3"/>
+      <c r="T20" s="21"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="8"/>
+      <c r="W20" s="20"/>
+      <c r="X20" s="3"/>
+      <c r="Y20" s="21"/>
+      <c r="Z20" s="20"/>
+      <c r="AA20" s="3"/>
+      <c r="AB20" s="3"/>
+      <c r="AC20" s="21"/>
+      <c r="AD20" s="8"/>
       <c r="AE20" s="8"/>
     </row>
     <row r="21" spans="1:31" x14ac:dyDescent="0.4">

</xml_diff>